<commit_message>
Set table definition column type from int to integer (like in FHIR)
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\uc-phep\interpolar\R-kds2db\kds2db\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\uc-phep\interpolar\R-cds2db\cds2db\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1070BF8-E8DA-45AE-82AE-7DB60B5F20CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF96DB8-C7B6-4B50-B508-3F7398E34D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="621" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>diagnosis/rank</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>hospitalization/admitSource/CodeableConcept</t>
   </si>
   <si>
@@ -786,9 +783,6 @@
     <t>repeat/offset</t>
   </si>
   <si>
-    <t>datatypes</t>
-  </si>
-  <si>
     <t xml:space="preserve">string </t>
   </si>
   <si>
@@ -796,6 +790,12 @@
   </si>
   <si>
     <t>Diese Tabelle enthält die in der Spalte type auswählbaren Datentypen</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>fhir_datatypes</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1266,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G247"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1415,7 +1417,7 @@
         <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>249</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -1426,20 +1428,20 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
         <v>28</v>
-      </c>
-      <c r="D22" t="s">
-        <v>29</v>
       </c>
       <c r="G22">
         <v>2</v>
@@ -1447,7 +1449,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -1458,7 +1460,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24">
         <v>2</v>
@@ -1466,15 +1468,15 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
         <v>33</v>
-      </c>
-      <c r="B27" t="s">
-        <v>34</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
@@ -1493,7 +1495,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F29">
         <v>50</v>
@@ -1504,7 +1506,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F30">
         <v>50</v>
@@ -1515,7 +1517,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F31">
         <v>10</v>
@@ -1523,10 +1525,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" t="s">
         <v>38</v>
-      </c>
-      <c r="E32" t="s">
-        <v>39</v>
       </c>
       <c r="F32">
         <v>30</v>
@@ -1534,7 +1536,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F33">
         <v>10</v>
@@ -1545,10 +1547,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
         <v>41</v>
-      </c>
-      <c r="B35" t="s">
-        <v>42</v>
       </c>
       <c r="C35" t="s">
         <v>13</v>
@@ -1559,7 +1561,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F36">
         <v>70</v>
@@ -1583,17 +1585,17 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G41">
         <v>2</v>
@@ -1601,17 +1603,17 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G44">
         <v>3</v>
@@ -1619,15 +1621,15 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" t="s">
         <v>51</v>
-      </c>
-      <c r="E46" t="s">
-        <v>52</v>
       </c>
       <c r="F46">
         <v>30</v>
@@ -1635,10 +1637,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F47">
         <v>30</v>
@@ -1646,22 +1648,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F51">
         <v>300</v>
@@ -1669,10 +1671,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F52">
         <v>30</v>
@@ -1680,17 +1682,17 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G55">
         <v>2</v>
@@ -1698,7 +1700,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G56">
         <v>4</v>
@@ -1706,7 +1708,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G57">
         <v>2</v>
@@ -1714,7 +1716,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G58">
         <v>2</v>
@@ -1722,10 +1724,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" t="s">
         <v>65</v>
-      </c>
-      <c r="B60" t="s">
-        <v>66</v>
       </c>
       <c r="C60" t="s">
         <v>13</v>
@@ -1744,7 +1746,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G62">
         <v>3</v>
@@ -1760,17 +1762,17 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G66">
         <v>15</v>
@@ -1778,7 +1780,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G67">
         <v>15</v>
@@ -1786,7 +1788,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G68">
         <v>15</v>
@@ -1794,10 +1796,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
+        <v>71</v>
+      </c>
+      <c r="E69" t="s">
         <v>72</v>
-      </c>
-      <c r="E69" t="s">
-        <v>73</v>
       </c>
       <c r="F69">
         <v>10</v>
@@ -1808,10 +1810,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" t="s">
         <v>74</v>
-      </c>
-      <c r="B71" t="s">
-        <v>75</v>
       </c>
       <c r="C71" t="s">
         <v>13</v>
@@ -1822,7 +1824,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F72">
         <v>70</v>
@@ -1846,10 +1848,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F75">
         <v>70</v>
@@ -1865,12 +1867,12 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F78">
         <v>20</v>
@@ -1878,7 +1880,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G79">
         <v>2</v>
@@ -1886,7 +1888,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F80">
         <v>10</v>
@@ -1894,10 +1896,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F81">
         <v>10</v>
@@ -1905,17 +1907,17 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G84">
         <v>2</v>
@@ -1923,10 +1925,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E85" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F85">
         <v>30</v>
@@ -1934,12 +1936,12 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G87">
         <v>2</v>
@@ -1947,7 +1949,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G88">
         <v>2</v>
@@ -1955,7 +1957,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G89">
         <v>2</v>
@@ -1963,7 +1965,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G90">
         <v>2</v>
@@ -1971,7 +1973,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G91">
         <v>2</v>
@@ -1979,15 +1981,15 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>90</v>
+      </c>
+      <c r="B94" t="s">
         <v>91</v>
-      </c>
-      <c r="B94" t="s">
-        <v>92</v>
       </c>
       <c r="C94" t="s">
         <v>13</v>
@@ -1998,7 +2000,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F95">
         <v>70</v>
@@ -2038,20 +2040,20 @@
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C100" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F102">
         <v>70</v>
@@ -2059,12 +2061,12 @@
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C103" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C104" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G104">
         <v>2</v>
@@ -2072,10 +2074,10 @@
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E105" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F105">
         <v>30</v>
@@ -2083,17 +2085,17 @@
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G108">
         <v>2</v>
@@ -2101,7 +2103,7 @@
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C109" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G109">
         <v>2</v>
@@ -2109,7 +2111,7 @@
     </row>
     <row r="110" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C110" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F110">
         <v>70</v>
@@ -2117,7 +2119,7 @@
     </row>
     <row r="111" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C111" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G111">
         <v>2</v>
@@ -2125,7 +2127,7 @@
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F112">
         <v>100</v>
@@ -2133,40 +2135,40 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C113" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C114" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C115" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C116" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C118" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>104</v>
+      </c>
+      <c r="B120" t="s">
         <v>105</v>
-      </c>
-      <c r="B120" t="s">
-        <v>106</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>13</v>
@@ -2187,7 +2189,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F122">
         <v>70</v>
@@ -2211,7 +2213,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C125" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D125" s="4"/>
       <c r="G125">
@@ -2228,20 +2230,20 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C127" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C128" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C129" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F129">
         <v>70</v>
@@ -2249,15 +2251,15 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C130" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C131" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E131" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F131">
         <v>30</v>
@@ -2265,16 +2267,16 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C132" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C133" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D133" s="3"/>
       <c r="E133" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F133">
         <v>30</v>
@@ -2282,24 +2284,24 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C134" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C135" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D135" s="3"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C136" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G137">
         <v>3</v>
@@ -2307,7 +2309,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G138">
         <v>2</v>
@@ -2315,7 +2317,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C139" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G139">
         <v>2</v>
@@ -2323,10 +2325,10 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>110</v>
+      </c>
+      <c r="B141" t="s">
         <v>111</v>
-      </c>
-      <c r="B141" t="s">
-        <v>112</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>13</v>
@@ -2338,7 +2340,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C142" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F142">
         <v>70</v>
@@ -2371,7 +2373,7 @@
     </row>
     <row r="146" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C146" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D146" s="4"/>
     </row>
@@ -2385,20 +2387,20 @@
     </row>
     <row r="148" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C148" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="149" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C149" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="150" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C150" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E150" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F150">
         <v>30</v>
@@ -2406,10 +2408,10 @@
     </row>
     <row r="151" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C151" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E151" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F151">
         <v>30</v>
@@ -2417,7 +2419,7 @@
     </row>
     <row r="152" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C152" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G152">
         <v>2</v>
@@ -2425,7 +2427,7 @@
     </row>
     <row r="153" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C153" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G153">
         <v>2</v>
@@ -2433,7 +2435,7 @@
     </row>
     <row r="154" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C154" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G154">
         <v>2</v>
@@ -2441,7 +2443,7 @@
     </row>
     <row r="155" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C155" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G155">
         <v>2</v>
@@ -2449,28 +2451,28 @@
     </row>
     <row r="156" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C156" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="157" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C157" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="158" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C158" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="159" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C159" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D159" s="3"/>
     </row>
     <row r="160" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G160">
         <v>3</v>
@@ -2478,7 +2480,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C161" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G161">
         <v>3</v>
@@ -2486,7 +2488,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C162" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G162">
         <v>3</v>
@@ -2494,7 +2496,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C163" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G163">
         <v>3</v>
@@ -2502,7 +2504,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C164" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G164">
         <v>3</v>
@@ -2510,7 +2512,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C165" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F165">
         <v>500</v>
@@ -2518,15 +2520,15 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C166" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
+        <v>127</v>
+      </c>
+      <c r="B168" t="s">
         <v>128</v>
-      </c>
-      <c r="B168" t="s">
-        <v>129</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>13</v>
@@ -2538,7 +2540,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C169" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F169">
         <v>70</v>
@@ -2571,7 +2573,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C173" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F173">
         <v>70</v>
@@ -2579,7 +2581,7 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C174" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F174">
         <v>70</v>
@@ -2595,22 +2597,22 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C176" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C177" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F177" s="3"/>
       <c r="G177" s="3"/>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C178" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E178" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F178">
         <v>30</v>
@@ -2618,10 +2620,10 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C179" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E179" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F179">
         <v>30</v>
@@ -2629,13 +2631,13 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C180" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D180" s="3"/>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C181" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F181">
         <v>500</v>
@@ -2643,15 +2645,15 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C182" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>133</v>
+      </c>
+      <c r="B184" t="s">
         <v>134</v>
-      </c>
-      <c r="B184" t="s">
-        <v>135</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>13</v>
@@ -2663,7 +2665,7 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C185" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F185">
         <v>70</v>
@@ -2688,7 +2690,7 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C188" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D188" s="4"/>
     </row>
@@ -2702,7 +2704,7 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C190" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F190">
         <v>30</v>
@@ -2710,20 +2712,20 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C191" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C192" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C193" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E193" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F193">
         <v>30</v>
@@ -2731,27 +2733,27 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C194" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D194" s="3"/>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C195" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D195" s="3"/>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C196" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>137</v>
+      </c>
+      <c r="B198" t="s">
         <v>138</v>
-      </c>
-      <c r="B198" t="s">
-        <v>139</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>13</v>
@@ -2763,7 +2765,7 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C199" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F199">
         <v>70</v>
@@ -2796,7 +2798,7 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C203" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D203" s="4"/>
     </row>
@@ -2810,25 +2812,25 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C205" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C206" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C207" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C208" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E208" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F208">
         <v>30</v>
@@ -2836,22 +2838,22 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C209" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C210" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C211" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C212" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G212">
         <v>2</v>
@@ -2859,10 +2861,10 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
+        <v>141</v>
+      </c>
+      <c r="B214" t="s">
         <v>142</v>
-      </c>
-      <c r="B214" t="s">
-        <v>143</v>
       </c>
       <c r="C214" s="3" t="s">
         <v>13</v>
@@ -2874,7 +2876,7 @@
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C215" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F215">
         <v>70</v>
@@ -2899,15 +2901,15 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C218" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C219" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E219" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F219">
         <v>30</v>
@@ -2915,7 +2917,7 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C220" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F220">
         <v>10</v>
@@ -2923,30 +2925,30 @@
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C221" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C222" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C223" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C224" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B226" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C226" t="s">
         <v>13</v>
@@ -2974,7 +2976,7 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C229" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F229">
         <v>50</v>
@@ -2982,7 +2984,7 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C230" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F230">
         <v>50</v>
@@ -2990,7 +2992,7 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C231" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F231">
         <v>30</v>
@@ -3001,13 +3003,13 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
+        <v>155</v>
+      </c>
+      <c r="C233" t="s">
         <v>156</v>
       </c>
-      <c r="C233" t="s">
-        <v>157</v>
-      </c>
       <c r="E233" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F233">
         <v>30</v>
@@ -3015,7 +3017,7 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C234" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F234">
         <v>30</v>
@@ -3023,7 +3025,7 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C235" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F235">
         <v>70</v>
@@ -3031,96 +3033,96 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B241" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B242" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B242" s="5" t="s">
+      <c r="E242" t="s">
         <v>167</v>
-      </c>
-      <c r="E242" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B243" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B243" s="5" t="s">
+      <c r="E243" t="s">
         <v>170</v>
-      </c>
-      <c r="E243" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B244" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B244" s="5" t="s">
+      <c r="E244" t="s">
         <v>173</v>
-      </c>
-      <c r="E244" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B245" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B245" s="5" t="s">
+      <c r="E245" t="s">
         <v>176</v>
-      </c>
-      <c r="E245" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B246" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B246" s="5" t="s">
+      <c r="E246" t="s">
         <v>179</v>
-      </c>
-      <c r="E246" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B247" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B247" s="5" t="s">
+      <c r="E247" t="s">
         <v>182</v>
-      </c>
-      <c r="E247" t="s">
-        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -3165,10 +3167,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" t="s">
         <v>199</v>
-      </c>
-      <c r="B2" t="s">
-        <v>200</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -3176,7 +3178,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -3184,7 +3186,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3192,7 +3194,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3200,7 +3202,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -3240,7 +3242,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -3251,7 +3253,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -3259,10 +3261,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3270,7 +3272,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C5">
         <v>5000</v>
@@ -3310,12 +3312,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3352,10 +3354,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" t="s">
         <v>199</v>
-      </c>
-      <c r="B2" t="s">
-        <v>200</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -3363,7 +3365,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -3371,7 +3373,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3379,7 +3381,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3387,7 +3389,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -3404,7 +3406,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3429,10 +3431,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>249</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -3440,7 +3442,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C3">
         <v>500</v>
@@ -3448,7 +3450,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -3456,7 +3458,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -3464,15 +3466,15 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -3480,67 +3482,67 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3554,7 +3556,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3579,10 +3581,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -3593,25 +3595,25 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>249</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -3619,10 +3621,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>249</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -3630,10 +3632,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -3641,10 +3643,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -3652,7 +3654,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -3660,10 +3662,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>249</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -3671,10 +3673,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>249</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -3682,10 +3684,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -3693,10 +3695,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -3704,7 +3706,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -3712,7 +3714,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -3723,10 +3725,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -3737,7 +3739,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C18">
         <v>20</v>
@@ -3748,10 +3750,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>249</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -3759,7 +3761,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3773,55 +3775,58 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3860,7 +3865,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -3868,12 +3873,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C4">
         <v>70</v>
@@ -3881,7 +3886,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3889,7 +3894,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3926,7 +3931,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2">
         <v>70</v>
@@ -3942,7 +3947,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3950,12 +3955,12 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -3997,7 +4002,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -4005,7 +4010,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C3">
         <v>500</v>
@@ -4048,7 +4053,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2">
         <v>70</v>
@@ -4056,7 +4061,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -4064,7 +4069,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -4072,7 +4077,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -4108,10 +4113,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -4119,10 +4124,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -4161,10 +4166,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" t="s">
         <v>199</v>
-      </c>
-      <c r="B2" t="s">
-        <v>200</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -4172,7 +4177,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -4180,7 +4185,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -4188,7 +4193,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -4196,7 +4201,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -4236,12 +4241,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -4278,10 +4283,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" t="s">
         <v>199</v>
-      </c>
-      <c r="B2" t="s">
-        <v>200</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -4289,7 +4294,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -4297,7 +4302,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C4">
         <v>70</v>
@@ -4305,7 +4310,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5">
         <v>30</v>

</xml_diff>

<commit_message>
Add Patient.name.text to TableDescription
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\uc-phep\interpolar\R-cds2db\cds2db\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF96DB8-C7B6-4B50-B508-3F7398E34D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAD90F7-4516-4893-B35F-818657753E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="621" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,16 +19,17 @@
     <sheet name="CodeableConcept" sheetId="4" r:id="rId4"/>
     <sheet name="Coding" sheetId="5" r:id="rId5"/>
     <sheet name="Period" sheetId="6" r:id="rId6"/>
-    <sheet name="Age" sheetId="7" r:id="rId7"/>
-    <sheet name="Range" sheetId="8" r:id="rId8"/>
-    <sheet name="SimpleQuantity" sheetId="9" r:id="rId9"/>
-    <sheet name="Duration" sheetId="10" r:id="rId10"/>
-    <sheet name="Annotation" sheetId="11" r:id="rId11"/>
-    <sheet name="Ratio" sheetId="12" r:id="rId12"/>
-    <sheet name="Quantity" sheetId="13" r:id="rId13"/>
-    <sheet name="Dosage" sheetId="14" r:id="rId14"/>
-    <sheet name="Timing" sheetId="15" r:id="rId15"/>
-    <sheet name="Datatypes" sheetId="16" r:id="rId16"/>
+    <sheet name="HumanName" sheetId="17" r:id="rId7"/>
+    <sheet name="Age" sheetId="7" r:id="rId8"/>
+    <sheet name="Range" sheetId="8" r:id="rId9"/>
+    <sheet name="SimpleQuantity" sheetId="9" r:id="rId10"/>
+    <sheet name="Duration" sheetId="10" r:id="rId11"/>
+    <sheet name="Annotation" sheetId="11" r:id="rId12"/>
+    <sheet name="Ratio" sheetId="12" r:id="rId13"/>
+    <sheet name="Quantity" sheetId="13" r:id="rId14"/>
+    <sheet name="Dosage" sheetId="14" r:id="rId15"/>
+    <sheet name="Timing" sheetId="15" r:id="rId16"/>
+    <sheet name="Datatypes" sheetId="16" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">table_description_collapsed!$F$8:$G$12</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="253">
   <si>
     <t>resource</t>
   </si>
@@ -147,12 +148,6 @@
     <t>pat</t>
   </si>
   <si>
-    <t>name/given</t>
-  </si>
-  <si>
-    <t>name/family</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -796,6 +791,18 @@
   </si>
   <si>
     <t>fhir_datatypes</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>given</t>
+  </si>
+  <si>
+    <t>name/HumanName</t>
   </si>
 </sst>
 </file>
@@ -838,7 +845,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,6 +864,12 @@
         <bgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -871,7 +884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -881,6 +894,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Good" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1264,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G247"/>
+  <dimension ref="A1:G246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,7 +1431,7 @@
         <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -1495,10 +1509,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29">
-        <v>50</v>
+        <v>252</v>
       </c>
       <c r="G29">
         <v>2</v>
@@ -1506,54 +1517,51 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F30">
-        <v>50</v>
-      </c>
-      <c r="G30">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
         <v>36</v>
       </c>
       <c r="F31">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>37</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32">
+        <v>10</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>38</v>
       </c>
-      <c r="F32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="B34" t="s">
         <v>39</v>
       </c>
-      <c r="F33">
-        <v>10</v>
-      </c>
-      <c r="G33">
-        <v>3</v>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34">
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C35" t="s">
         <v>40</v>
-      </c>
-      <c r="B35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" t="s">
-        <v>13</v>
       </c>
       <c r="F35">
         <v>70</v>
@@ -1561,7 +1569,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="F36">
         <v>70</v>
@@ -1569,59 +1577,62 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37">
-        <v>70</v>
+        <v>16</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>45</v>
-      </c>
-      <c r="G41">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>48</v>
-      </c>
-      <c r="G44">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" t="s">
         <v>49</v>
+      </c>
+      <c r="F45">
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1629,7 +1640,7 @@
         <v>50</v>
       </c>
       <c r="E46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F46">
         <v>30</v>
@@ -1637,142 +1648,139 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>52</v>
-      </c>
-      <c r="E47" t="s">
         <v>51</v>
-      </c>
-      <c r="F47">
-        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="F50">
+        <v>300</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="E51" t="s">
+        <v>49</v>
       </c>
       <c r="F51">
-        <v>300</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>57</v>
-      </c>
-      <c r="E52" t="s">
-        <v>51</v>
-      </c>
-      <c r="F52">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G55">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G56">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
+        <v>61</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>62</v>
       </c>
-      <c r="G57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
+      <c r="B59" t="s">
         <v>63</v>
       </c>
-      <c r="G58">
-        <v>2</v>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59">
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>64</v>
-      </c>
-      <c r="B60" t="s">
-        <v>65</v>
-      </c>
       <c r="C60" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60">
-        <v>70</v>
+        <v>16</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G61">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>47</v>
-      </c>
-      <c r="G62">
-        <v>3</v>
+        <v>17</v>
+      </c>
+      <c r="F62">
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>17</v>
-      </c>
-      <c r="F63">
-        <v>20</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="G65">
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G66">
         <v>15</v>
@@ -1780,7 +1788,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G67">
         <v>15</v>
@@ -1788,35 +1796,35 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="E68" t="s">
+        <v>70</v>
+      </c>
+      <c r="F68">
+        <v>10</v>
       </c>
       <c r="G68">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>71</v>
       </c>
-      <c r="E69" t="s">
+      <c r="B70" t="s">
         <v>72</v>
       </c>
-      <c r="F69">
-        <v>10</v>
-      </c>
-      <c r="G69">
-        <v>15</v>
+      <c r="C70" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70">
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>73</v>
-      </c>
-      <c r="B71" t="s">
-        <v>74</v>
-      </c>
       <c r="C71" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F71">
         <v>70</v>
@@ -1824,7 +1832,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="F72">
         <v>70</v>
@@ -1832,63 +1840,66 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73">
-        <v>70</v>
+        <v>16</v>
+      </c>
+      <c r="G73">
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>16</v>
-      </c>
-      <c r="G74">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="D74" t="s">
+        <v>62</v>
+      </c>
+      <c r="F74">
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>75</v>
-      </c>
-      <c r="D75" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="F75">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>17</v>
-      </c>
-      <c r="F76">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="F77">
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>77</v>
-      </c>
-      <c r="F78">
-        <v>20</v>
+        <v>43</v>
+      </c>
+      <c r="G78">
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>45</v>
-      </c>
-      <c r="G79">
-        <v>2</v>
+        <v>76</v>
+      </c>
+      <c r="F79">
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="E80" t="s">
+        <v>70</v>
       </c>
       <c r="F80">
         <v>10</v>
@@ -1896,52 +1907,49 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>79</v>
-      </c>
-      <c r="E81" t="s">
-        <v>72</v>
-      </c>
-      <c r="F81">
-        <v>10</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>82</v>
-      </c>
-      <c r="G84">
-        <v>2</v>
+        <v>81</v>
+      </c>
+      <c r="E84" t="s">
+        <v>49</v>
+      </c>
+      <c r="F84">
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>83</v>
-      </c>
-      <c r="E85" t="s">
-        <v>51</v>
-      </c>
-      <c r="F85">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="G86">
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G87">
         <v>2</v>
@@ -1949,7 +1957,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G88">
         <v>2</v>
@@ -1957,7 +1965,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="G89">
         <v>2</v>
@@ -1965,7 +1973,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="G90">
         <v>2</v>
@@ -1973,26 +1981,26 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>88</v>
       </c>
-      <c r="G91">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C92" t="s">
+      <c r="B93" t="s">
         <v>89</v>
       </c>
+      <c r="C93" t="s">
+        <v>13</v>
+      </c>
+      <c r="F93">
+        <v>70</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="C94" t="s">
         <v>90</v>
-      </c>
-      <c r="B94" t="s">
-        <v>91</v>
-      </c>
-      <c r="C94" t="s">
-        <v>13</v>
       </c>
       <c r="F94">
         <v>70</v>
@@ -2000,7 +2008,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="F95">
         <v>70</v>
@@ -2008,7 +2016,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F96">
         <v>70</v>
@@ -2016,86 +2024,86 @@
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
-        <v>15</v>
-      </c>
-      <c r="F97">
-        <v>70</v>
+        <v>16</v>
+      </c>
+      <c r="G97">
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
-        <v>16</v>
-      </c>
-      <c r="G98">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="F98">
+        <v>30</v>
       </c>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
-        <v>17</v>
-      </c>
-      <c r="F99">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C100" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
-        <v>45</v>
+        <v>73</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F101">
+        <v>70</v>
       </c>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
-        <v>75</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F102">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C103" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="G103">
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C104" t="s">
-        <v>82</v>
-      </c>
-      <c r="G104">
-        <v>2</v>
+        <v>91</v>
+      </c>
+      <c r="E104" t="s">
+        <v>49</v>
+      </c>
+      <c r="F104">
+        <v>30</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
-        <v>93</v>
-      </c>
-      <c r="E105" t="s">
-        <v>51</v>
-      </c>
-      <c r="F105">
-        <v>30</v>
+        <v>92</v>
       </c>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
-        <v>95</v>
+        <v>83</v>
+      </c>
+      <c r="G107">
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G108">
         <v>2</v>
@@ -2103,93 +2111,93 @@
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C109" t="s">
-        <v>86</v>
-      </c>
-      <c r="G109">
-        <v>2</v>
+        <v>94</v>
+      </c>
+      <c r="F109">
+        <v>70</v>
       </c>
     </row>
     <row r="110" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C110" t="s">
-        <v>96</v>
-      </c>
-      <c r="F110">
-        <v>70</v>
+        <v>61</v>
+      </c>
+      <c r="G110">
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C111" t="s">
-        <v>63</v>
-      </c>
-      <c r="G111">
-        <v>2</v>
+        <v>95</v>
+      </c>
+      <c r="F111">
+        <v>100</v>
       </c>
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
-        <v>97</v>
-      </c>
-      <c r="F112">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C113" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C114" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C115" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C116" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C118" t="s">
+      <c r="B119" t="s">
         <v>103</v>
       </c>
+      <c r="C119" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D119" s="3"/>
+      <c r="F119">
+        <v>70</v>
+      </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>104</v>
-      </c>
-      <c r="B120" t="s">
-        <v>105</v>
-      </c>
       <c r="C120" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D120" s="3"/>
-      <c r="F120">
-        <v>70</v>
+      <c r="G120">
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C121" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D121" s="3"/>
-      <c r="G121">
-        <v>2</v>
+      <c r="C121" t="s">
+        <v>90</v>
+      </c>
+      <c r="F121">
+        <v>70</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="F122">
         <v>70</v>
@@ -2197,150 +2205,150 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F123">
         <v>70</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C124" t="s">
-        <v>15</v>
-      </c>
-      <c r="F124">
-        <v>70</v>
+      <c r="C124" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D124" s="4"/>
+      <c r="G124">
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C125" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D125" s="4"/>
-      <c r="G125">
-        <v>2</v>
+      <c r="C125" t="s">
+        <v>17</v>
+      </c>
+      <c r="F125">
+        <v>30</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
-        <v>17</v>
-      </c>
-      <c r="F126">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C127" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C128" t="s">
-        <v>45</v>
+        <v>73</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F128">
+        <v>70</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C129" t="s">
-        <v>75</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F129">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C130" t="s">
-        <v>81</v>
+        <v>91</v>
+      </c>
+      <c r="E130" t="s">
+        <v>49</v>
+      </c>
+      <c r="F130">
+        <v>30</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C131" t="s">
-        <v>93</v>
-      </c>
-      <c r="E131" t="s">
-        <v>51</v>
-      </c>
-      <c r="F131">
-        <v>30</v>
+        <v>92</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C132" t="s">
-        <v>94</v>
+      <c r="C132" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D132" s="3"/>
+      <c r="E132" t="s">
+        <v>49</v>
+      </c>
+      <c r="F132">
+        <v>30</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C133" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D133" s="3"/>
-      <c r="E133" t="s">
-        <v>51</v>
-      </c>
-      <c r="F133">
-        <v>30</v>
-      </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C134" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C135" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D135" s="3"/>
+      <c r="C135" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C136" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="G136">
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="G137">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="G138">
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C139" t="s">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>108</v>
+      </c>
+      <c r="B140" t="s">
         <v>109</v>
       </c>
-      <c r="G139">
-        <v>2</v>
+      <c r="C140" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D140" s="3"/>
+      <c r="F140">
+        <v>70</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>110</v>
-      </c>
-      <c r="B141" t="s">
-        <v>111</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D141" s="3"/>
+      <c r="C141" t="s">
+        <v>40</v>
+      </c>
       <c r="F141">
         <v>70</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C142" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="F142">
         <v>70</v>
@@ -2348,41 +2356,38 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C143" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F143">
         <v>70</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C144" t="s">
-        <v>15</v>
-      </c>
-      <c r="F144">
-        <v>70</v>
+      <c r="C144" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D144" s="3"/>
+      <c r="G144">
+        <v>2</v>
       </c>
     </row>
     <row r="145" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C145" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D145" s="3"/>
-      <c r="G145">
-        <v>2</v>
-      </c>
+      <c r="C145" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D145" s="4"/>
     </row>
     <row r="146" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C146" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D146" s="4"/>
+      <c r="C146" t="s">
+        <v>17</v>
+      </c>
+      <c r="F146">
+        <v>30</v>
+      </c>
     </row>
     <row r="147" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C147" t="s">
-        <v>17</v>
-      </c>
-      <c r="F147">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="148" spans="3:7" x14ac:dyDescent="0.25">
@@ -2392,15 +2397,21 @@
     </row>
     <row r="149" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C149" t="s">
-        <v>47</v>
+        <v>91</v>
+      </c>
+      <c r="E149" t="s">
+        <v>49</v>
+      </c>
+      <c r="F149">
+        <v>30</v>
       </c>
     </row>
     <row r="150" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C150" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E150" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F150">
         <v>30</v>
@@ -2408,18 +2419,15 @@
     </row>
     <row r="151" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C151" t="s">
-        <v>112</v>
-      </c>
-      <c r="E151" t="s">
-        <v>51</v>
-      </c>
-      <c r="F151">
-        <v>30</v>
+        <v>111</v>
+      </c>
+      <c r="G151">
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C152" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G152">
         <v>2</v>
@@ -2427,7 +2435,7 @@
     </row>
     <row r="153" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C153" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G153">
         <v>2</v>
@@ -2435,7 +2443,7 @@
     </row>
     <row r="154" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C154" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G154">
         <v>2</v>
@@ -2443,36 +2451,36 @@
     </row>
     <row r="155" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C155" t="s">
-        <v>116</v>
-      </c>
-      <c r="G155">
-        <v>2</v>
+        <v>115</v>
       </c>
     </row>
     <row r="156" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C156" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
     </row>
     <row r="157" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C157" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
     </row>
     <row r="158" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C158" t="s">
+      <c r="C158" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D158" s="3"/>
+    </row>
+    <row r="159" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C159" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="159" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C159" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D159" s="3"/>
+      <c r="G159">
+        <v>3</v>
+      </c>
     </row>
     <row r="160" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G160">
         <v>3</v>
@@ -2480,7 +2488,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C161" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G161">
         <v>3</v>
@@ -2488,7 +2496,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C162" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G162">
         <v>3</v>
@@ -2496,7 +2504,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C163" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G163">
         <v>3</v>
@@ -2504,43 +2512,43 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C164" t="s">
-        <v>124</v>
-      </c>
-      <c r="G164">
-        <v>3</v>
+        <v>123</v>
+      </c>
+      <c r="F164">
+        <v>500</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C165" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>125</v>
       </c>
-      <c r="F165">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C166" t="s">
+      <c r="B167" t="s">
         <v>126</v>
       </c>
+      <c r="C167" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D167" s="3"/>
+      <c r="F167">
+        <v>70</v>
+      </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>127</v>
-      </c>
-      <c r="B168" t="s">
-        <v>128</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D168" s="3"/>
+      <c r="C168" t="s">
+        <v>40</v>
+      </c>
       <c r="F168">
         <v>70</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C169" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="F169">
         <v>70</v>
@@ -2548,32 +2556,32 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C170" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F170">
         <v>70</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C171" t="s">
-        <v>15</v>
-      </c>
-      <c r="F171">
-        <v>70</v>
+      <c r="C171" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D171" s="3"/>
+      <c r="G171">
+        <v>2</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C172" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D172" s="3"/>
-      <c r="G172">
-        <v>2</v>
+      <c r="C172" t="s">
+        <v>127</v>
+      </c>
+      <c r="F172">
+        <v>70</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C173" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F173">
         <v>70</v>
@@ -2581,122 +2589,122 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C174" t="s">
-        <v>130</v>
+        <v>17</v>
       </c>
       <c r="F174">
-        <v>70</v>
+        <v>30</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C175" t="s">
-        <v>17</v>
-      </c>
-      <c r="F175">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C176" t="s">
         <v>45</v>
       </c>
+      <c r="F176" s="3"/>
+      <c r="G176" s="3"/>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C177" t="s">
-        <v>47</v>
-      </c>
-      <c r="F177" s="3"/>
-      <c r="G177" s="3"/>
+        <v>91</v>
+      </c>
+      <c r="E177" t="s">
+        <v>49</v>
+      </c>
+      <c r="F177">
+        <v>30</v>
+      </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C178" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E178" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F178">
         <v>30</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C179" t="s">
-        <v>112</v>
-      </c>
-      <c r="E179" t="s">
-        <v>51</v>
-      </c>
-      <c r="F179">
-        <v>30</v>
-      </c>
+      <c r="C179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D179" s="3"/>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C180" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D180" s="3"/>
+      <c r="C180" t="s">
+        <v>129</v>
+      </c>
+      <c r="F180">
+        <v>500</v>
+      </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C181" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>131</v>
       </c>
-      <c r="F181">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C182" t="s">
+      <c r="B183" t="s">
         <v>132</v>
       </c>
+      <c r="C183" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D183" s="3"/>
+      <c r="F183">
+        <v>70</v>
+      </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>133</v>
-      </c>
-      <c r="B184" t="s">
-        <v>134</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D184" s="3"/>
+      <c r="C184" t="s">
+        <v>40</v>
+      </c>
       <c r="F184">
         <v>70</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C185" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="F185">
         <v>70</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C186" t="s">
-        <v>14</v>
-      </c>
-      <c r="F186">
-        <v>70</v>
+      <c r="C186" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D186" s="3"/>
+      <c r="G186">
+        <v>2</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C187" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D187" s="3"/>
-      <c r="G187">
-        <v>2</v>
-      </c>
+      <c r="C187" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D187" s="4"/>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C188" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D188" s="4"/>
+      <c r="C188" t="s">
+        <v>17</v>
+      </c>
+      <c r="F188">
+        <v>30</v>
+      </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C189" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="F189">
         <v>30</v>
@@ -2704,10 +2712,7 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C190" t="s">
-        <v>135</v>
-      </c>
-      <c r="F190">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -2717,55 +2722,58 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C192" t="s">
-        <v>47</v>
+        <v>81</v>
+      </c>
+      <c r="E192" t="s">
+        <v>49</v>
+      </c>
+      <c r="F192">
+        <v>30</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C193" t="s">
-        <v>83</v>
-      </c>
-      <c r="E193" t="s">
-        <v>51</v>
-      </c>
-      <c r="F193">
-        <v>30</v>
-      </c>
+      <c r="C193" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D193" s="3"/>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C194" s="3" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="D194" s="3"/>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C195" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D195" s="3"/>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C196" t="s">
+      <c r="C195" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>135</v>
+      </c>
+      <c r="B197" t="s">
         <v>136</v>
       </c>
+      <c r="C197" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D197" s="3"/>
+      <c r="F197">
+        <v>70</v>
+      </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>137</v>
-      </c>
-      <c r="B198" t="s">
-        <v>138</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D198" s="3"/>
+      <c r="C198" t="s">
+        <v>40</v>
+      </c>
       <c r="F198">
         <v>70</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C199" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="F199">
         <v>70</v>
@@ -2773,46 +2781,43 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C200" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F200">
         <v>70</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C201" t="s">
-        <v>15</v>
-      </c>
-      <c r="F201">
-        <v>70</v>
+      <c r="C201" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D201" s="3"/>
+      <c r="G201">
+        <v>2</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C202" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D202" s="3"/>
-      <c r="G202">
-        <v>2</v>
-      </c>
+      <c r="C202" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D202" s="4"/>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C203" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D203" s="4"/>
+      <c r="C203" t="s">
+        <v>17</v>
+      </c>
+      <c r="F203">
+        <v>30</v>
+      </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C204" t="s">
-        <v>17</v>
-      </c>
-      <c r="F204">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C205" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -2822,161 +2827,164 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C207" t="s">
-        <v>47</v>
+        <v>137</v>
+      </c>
+      <c r="E207" t="s">
+        <v>49</v>
+      </c>
+      <c r="F207">
+        <v>30</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C208" t="s">
-        <v>139</v>
-      </c>
-      <c r="E208" t="s">
-        <v>51</v>
-      </c>
-      <c r="F208">
-        <v>30</v>
+        <v>138</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C209" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C210" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C211" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C212" t="s">
-        <v>63</v>
-      </c>
-      <c r="G212">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="G211">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>139</v>
+      </c>
+      <c r="B213" t="s">
+        <v>140</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D213" s="3"/>
+      <c r="F213">
+        <v>70</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+      <c r="C214" t="s">
         <v>141</v>
       </c>
-      <c r="B214" t="s">
-        <v>142</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D214" s="3"/>
       <c r="F214">
         <v>70</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C215" t="s">
-        <v>143</v>
-      </c>
-      <c r="F215">
-        <v>70</v>
+      <c r="C215" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D215" s="3"/>
+      <c r="G215">
+        <v>2</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C216" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D216" s="3"/>
-      <c r="G216">
-        <v>2</v>
+      <c r="C216" t="s">
+        <v>17</v>
+      </c>
+      <c r="F216">
+        <v>30</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C217" t="s">
-        <v>17</v>
-      </c>
-      <c r="F217">
-        <v>30</v>
+        <v>142</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C218" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+      <c r="E218" t="s">
+        <v>49</v>
+      </c>
+      <c r="F218">
+        <v>30</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C219" t="s">
-        <v>145</v>
-      </c>
-      <c r="E219" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
       <c r="F219">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C220" t="s">
-        <v>146</v>
-      </c>
-      <c r="F220">
-        <v>10</v>
+        <v>145</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C221" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C222" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C223" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>28</v>
+      </c>
+      <c r="B225" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C224" t="s">
-        <v>150</v>
+      <c r="C225" t="s">
+        <v>13</v>
+      </c>
+      <c r="F225">
+        <v>70</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>28</v>
-      </c>
-      <c r="B226" t="s">
-        <v>151</v>
-      </c>
-      <c r="C226" t="s">
-        <v>13</v>
-      </c>
-      <c r="F226">
-        <v>70</v>
+      <c r="C226" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D226" s="3"/>
+      <c r="G226">
+        <v>2</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C227" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D227" s="3"/>
-      <c r="G227">
-        <v>2</v>
+      <c r="C227" t="s">
+        <v>17</v>
+      </c>
+      <c r="F227">
+        <v>30</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C228" t="s">
-        <v>17</v>
+        <v>150</v>
       </c>
       <c r="F228">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C229" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F229">
         <v>50</v>
@@ -2984,32 +2992,32 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C230" t="s">
+        <v>152</v>
+      </c>
+      <c r="F230">
+        <v>30</v>
+      </c>
+      <c r="G230">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
         <v>153</v>
       </c>
-      <c r="F230">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C231" t="s">
+      <c r="C232" t="s">
         <v>154</v>
       </c>
-      <c r="F231">
-        <v>30</v>
-      </c>
-      <c r="G231">
-        <v>3</v>
+      <c r="E232" t="s">
+        <v>49</v>
+      </c>
+      <c r="F232">
+        <v>30</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
+      <c r="C233" t="s">
         <v>155</v>
-      </c>
-      <c r="C233" t="s">
-        <v>156</v>
-      </c>
-      <c r="E233" t="s">
-        <v>51</v>
       </c>
       <c r="F233">
         <v>30</v>
@@ -3017,112 +3025,104 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C234" t="s">
+        <v>156</v>
+      </c>
+      <c r="F234">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
         <v>157</v>
-      </c>
-      <c r="F234">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C235" t="s">
-        <v>158</v>
-      </c>
-      <c r="F235">
-        <v>70</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
+      <c r="B240" s="1" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
+      <c r="A241" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B241" s="1" t="s">
+      <c r="B241" s="5" t="s">
         <v>164</v>
+      </c>
+      <c r="E241" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E242" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E243" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E244" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E245" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E246" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A247" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="B247" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="E247" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3135,7 +3135,7 @@
           <x14:formula1>
             <xm:f>Datatypes!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>E8:E235</xm:sqref>
+          <xm:sqref>E8:E234</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3144,6 +3144,73 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -3167,10 +3234,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -3178,7 +3245,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -3186,7 +3253,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3194,7 +3261,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3202,7 +3269,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -3214,7 +3281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3242,7 +3309,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -3253,7 +3320,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -3261,10 +3328,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3272,7 +3339,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C5">
         <v>5000</v>
@@ -3284,7 +3351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3312,12 +3379,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3326,7 +3393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -3354,10 +3421,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -3365,7 +3432,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -3373,7 +3440,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3381,7 +3448,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3389,7 +3456,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -3401,7 +3468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -3431,10 +3498,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -3442,7 +3509,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C3">
         <v>500</v>
@@ -3450,7 +3517,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -3458,7 +3525,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -3466,15 +3533,15 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -3482,67 +3549,67 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3551,7 +3618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -3581,10 +3648,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -3595,25 +3662,25 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -3621,10 +3688,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -3632,10 +3699,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -3643,10 +3710,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -3654,7 +3721,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -3662,10 +3729,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -3673,10 +3740,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -3684,10 +3751,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -3695,10 +3762,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -3706,7 +3773,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -3714,7 +3781,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -3725,10 +3792,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -3739,7 +3806,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C18">
         <v>20</v>
@@ -3750,10 +3817,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -3761,7 +3828,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3770,7 +3837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671D09BB-E5B9-4217-A0D2-BB413AC8772B}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -3785,48 +3852,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3865,7 +3932,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -3873,12 +3940,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C4">
         <v>70</v>
@@ -3886,7 +3953,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3894,7 +3961,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3931,7 +3998,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C2">
         <v>70</v>
@@ -3947,7 +4014,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3955,12 +4022,12 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -4002,7 +4069,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -4010,7 +4077,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C3">
         <v>500</v>
@@ -4053,7 +4120,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C2">
         <v>70</v>
@@ -4061,7 +4128,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -4069,7 +4136,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -4077,7 +4144,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -4093,7 +4160,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4113,10 +4182,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -4124,10 +4193,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -4140,6 +4209,71 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283E0D1E-AFF3-4AC2-AF90-985385A50C24}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -4166,10 +4300,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -4177,7 +4311,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -4185,7 +4319,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -4193,7 +4327,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -4201,7 +4335,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -4213,7 +4347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -4241,79 +4375,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
         <v>203</v>
-      </c>
-      <c r="C5">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add generating Copy Fnction Scripts for Database
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\uc-phep\interpolar\R-cds2db\cds2db\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAD90F7-4516-4893-B35F-818657753E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE99091-6CBA-4BC0-8F93-80C592143198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="621" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1281,7 +1281,7 @@
   <dimension ref="A1:G246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4213,7 +4213,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove unnecessary string types in Table Description
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\uc-phep\interpolar\R-cds2db\cds2db\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FFC928-2820-47FB-A897-20A45D0A61FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9268FC27-2F66-4FD9-834F-38B32338C946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="621" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="252">
   <si>
     <t>resource</t>
   </si>
@@ -791,9 +791,6 @@
   </si>
   <si>
     <t>fhir_datatypes</t>
-  </si>
-  <si>
-    <t>string</t>
   </si>
   <si>
     <t>family</t>
@@ -1280,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,7 +1506,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G29">
         <v>2</v>
@@ -4213,7 +4210,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4236,18 +4233,12 @@
       <c r="A2" t="s">
         <v>189</v>
       </c>
-      <c r="B2" t="s">
-        <v>249</v>
-      </c>
       <c r="C2">
         <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>250</v>
-      </c>
-      <c r="B3" t="s">
         <v>249</v>
       </c>
       <c r="C3">
@@ -4256,10 +4247,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>251</v>
-      </c>
-      <c r="B4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C4">
         <v>30</v>

</xml_diff>

<commit_message>
Add deceasedDateTime in Table_Description and SQL scrips
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="254">
   <si>
     <t xml:space="preserve">RESOURCE</t>
   </si>
@@ -150,6 +150,12 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
+    <t xml:space="preserve">deceasedDateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime</t>
+  </si>
+  <si>
     <t xml:space="preserve">address/postalCode</t>
   </si>
   <si>
@@ -184,9 +190,6 @@
   </si>
   <si>
     <t xml:space="preserve">onsetDateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datetime</t>
   </si>
   <si>
     <t xml:space="preserve">abatementDateTime</t>
@@ -908,7 +911,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -919,6 +922,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1191,10 +1198,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G233"/>
+  <dimension ref="A1:G234"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C72" activeCellId="0" sqref="C72:G72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1420,39 +1427,42 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="1" t="s">
+    <row r="29" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="E29" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F29" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="G29" s="1" t="n">
+      <c r="G30" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="1" t="s">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F32" s="1" t="n">
-        <v>70</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F33" s="1" t="n">
         <v>70</v>
@@ -1460,54 +1470,51 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>13</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G36" s="1" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="G37" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G39" s="1" t="n">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F41" s="1" t="n">
-        <v>35</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1515,7 +1522,7 @@
         <v>50</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F42" s="1" t="n">
         <v>35</v>
@@ -1525,6 +1532,12 @@
       <c r="C43" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="E43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1" t="s">
@@ -1540,25 +1553,25 @@
       <c r="C46" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F46" s="1" t="n">
-        <v>300</v>
-      </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F47" s="1" t="n">
-        <v>35</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="E48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="s">
@@ -1569,16 +1582,13 @@
       <c r="C50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G50" s="1" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G51" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,7 +1596,7 @@
         <v>60</v>
       </c>
       <c r="G52" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,36 +1607,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="G54" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="B56" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G56" s="1" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F57" s="1" t="n">
-        <v>20</v>
+        <v>47</v>
+      </c>
+      <c r="G57" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="1" t="s">
-        <v>64</v>
+        <v>15</v>
+      </c>
+      <c r="F58" s="1" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,9 +1651,6 @@
       <c r="C60" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G60" s="1" t="n">
-        <v>15</v>
-      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="1" t="s">
@@ -1662,38 +1672,38 @@
       <c r="C63" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F63" s="1" t="n">
-        <v>10</v>
-      </c>
       <c r="G63" s="1" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="F64" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G64" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="B66" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F66" s="1" t="n">
-        <v>70</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F67" s="1" t="n">
         <v>70</v>
@@ -1701,10 +1711,7 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="F68" s="1" t="n">
         <v>70</v>
@@ -1712,24 +1719,27 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="1" t="s">
-        <v>15</v>
+        <v>74</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="F69" s="1" t="n">
-        <v>20</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="1" t="s">
-        <v>74</v>
+        <v>15</v>
+      </c>
+      <c r="F70" s="1" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F71" s="1" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="1" t="s">
@@ -1741,27 +1751,24 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G73" s="1" t="n">
-        <v>2</v>
+        <v>77</v>
+      </c>
+      <c r="F73" s="1" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F74" s="1" t="n">
-        <v>10</v>
+        <v>45</v>
+      </c>
+      <c r="G74" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E75" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="F75" s="1" t="n">
         <v>10</v>
       </c>
@@ -1770,6 +1777,12 @@
       <c r="C76" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="E76" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F76" s="1" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="1" t="s">
@@ -1780,33 +1793,30 @@
       <c r="C78" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G78" s="1" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F79" s="1" t="n">
-        <v>35</v>
+      <c r="G79" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="E80" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F80" s="1" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G81" s="1" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="1" t="s">
@@ -1826,7 +1836,7 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="1" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="G84" s="1" t="n">
         <v>2</v>
@@ -1834,7 +1844,7 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="1" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="G85" s="1" t="n">
         <v>2</v>
@@ -1844,29 +1854,29 @@
       <c r="C86" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
+      <c r="G86" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B88" s="1" t="s">
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="B89" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F89" s="1" t="n">
-        <v>70</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="F90" s="1" t="n">
         <v>70</v>
@@ -1874,7 +1884,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F91" s="1" t="n">
         <v>70</v>
@@ -1882,61 +1892,64 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F92" s="1" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="1" t="s">
-        <v>74</v>
+        <v>15</v>
+      </c>
+      <c r="F93" s="1" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="1" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F95" s="1" t="n">
-        <v>70</v>
+        <v>45</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F96" s="1" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G97" s="1" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F98" s="1" t="n">
-        <v>35</v>
+        <v>82</v>
+      </c>
+      <c r="G98" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="E99" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F99" s="1" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="1" t="s">
@@ -1945,10 +1958,7 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G101" s="1" t="n">
-        <v>2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1961,32 +1971,35 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F103" s="1" t="n">
-        <v>70</v>
+        <v>86</v>
+      </c>
+      <c r="G103" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G104" s="1" t="n">
-        <v>2</v>
+        <v>96</v>
+      </c>
+      <c r="F104" s="1" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F105" s="1" t="n">
-        <v>100</v>
+        <v>62</v>
+      </c>
+      <c r="G105" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="F106" s="1" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="1" t="s">
@@ -2013,29 +2026,26 @@
         <v>102</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="s">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C112" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B113" s="1" t="s">
+    </row>
+    <row r="114" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="B114" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C114" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D113" s="3"/>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C114" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F114" s="1" t="n">
-        <v>70</v>
-      </c>
+      <c r="D114" s="4"/>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="1" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="F115" s="1" t="n">
         <v>70</v>
@@ -2043,147 +2053,147 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F116" s="1" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C117" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D117" s="4"/>
-      <c r="G117" s="1" t="n">
-        <v>2</v>
+      <c r="C117" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F117" s="1" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F118" s="1" t="n">
-        <v>30</v>
+      <c r="C118" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D118" s="5"/>
+      <c r="G118" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C119" s="1" t="s">
-        <v>74</v>
+        <v>15</v>
+      </c>
+      <c r="F119" s="1" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C120" s="1" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F121" s="1" t="n">
-        <v>70</v>
+        <v>45</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C122" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F122" s="1" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F123" s="1" t="n">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="125" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C125" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D125" s="3"/>
-      <c r="E125" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F125" s="1" t="n">
+      <c r="E124" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F124" s="1" t="n">
         <v>35</v>
       </c>
     </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C125" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="126" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C126" s="3" t="s">
+      <c r="C126" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D126" s="3"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F126" s="1" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="3" t="s">
+      <c r="C127" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D127" s="3"/>
-    </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C128" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="D127" s="4"/>
+    </row>
+    <row r="128" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C128" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D128" s="4"/>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G129" s="1" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="1" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="G130" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="1" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="G131" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="s">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C132" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="G132" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C133" s="3" t="s">
+      <c r="B134" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C134" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D133" s="3"/>
-    </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C134" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F134" s="1" t="n">
-        <v>70</v>
-      </c>
+      <c r="D134" s="4"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F135" s="1" t="n">
         <v>70</v>
@@ -2191,29 +2201,32 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F136" s="1" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C137" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D137" s="4"/>
+      <c r="C137" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F137" s="1" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C138" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F138" s="1" t="n">
-        <v>30</v>
-      </c>
+      <c r="C138" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D138" s="5"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="F139" s="1" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,21 +2236,15 @@
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F141" s="1" t="n">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="1" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F142" s="1" t="n">
         <v>35</v>
@@ -2247,8 +2254,11 @@
       <c r="C143" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G143" s="1" t="n">
-        <v>2</v>
+      <c r="E143" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F143" s="1" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2279,30 +2289,30 @@
       <c r="C147" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="G147" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="1" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C149" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C150" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C150" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D150" s="3"/>
-    </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="1" t="s">
+    </row>
+    <row r="151" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C151" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="G151" s="1" t="n">
-        <v>3</v>
-      </c>
+      <c r="D151" s="4"/>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="1" t="s">
@@ -2340,38 +2350,38 @@
       <c r="C156" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F156" s="1" t="n">
-        <v>500</v>
+      <c r="G156" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="159" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="s">
+      <c r="F157" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C158" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B159" s="1" t="s">
+    </row>
+    <row r="160" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C159" s="3" t="s">
+      <c r="B160" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C160" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D159" s="3"/>
-    </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C160" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F160" s="1" t="n">
-        <v>70</v>
-      </c>
+      <c r="D160" s="4"/>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C161" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F161" s="1" t="n">
         <v>70</v>
@@ -2379,7 +2389,7 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C162" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F162" s="1" t="n">
         <v>70</v>
@@ -2387,7 +2397,7 @@
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C163" s="1" t="s">
-        <v>128</v>
+        <v>14</v>
       </c>
       <c r="F163" s="1" t="n">
         <v>70</v>
@@ -2403,110 +2413,110 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C165" s="1" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="F165" s="1" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="F166" s="1" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C167" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F167" s="3"/>
-      <c r="G167" s="3"/>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C168" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F168" s="1" t="n">
-        <v>35</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F168" s="4"/>
+      <c r="G168" s="4"/>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C169" s="1" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F169" s="1" t="n">
         <v>35</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C170" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D170" s="3"/>
-    </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C171" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F171" s="1" t="n">
-        <v>500</v>
-      </c>
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C170" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F170" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C171" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D171" s="4"/>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C172" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="174" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="1" t="s">
+      <c r="F172" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C173" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B174" s="1" t="s">
+    </row>
+    <row r="175" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C174" s="3" t="s">
+      <c r="B175" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C175" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D174" s="3"/>
-    </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C175" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F175" s="1" t="n">
-        <v>70</v>
-      </c>
+      <c r="D175" s="4"/>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C176" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F176" s="1" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C177" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D177" s="4"/>
+      <c r="C177" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F177" s="1" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F178" s="1" t="n">
-        <v>30</v>
-      </c>
+      <c r="C178" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D178" s="5"/>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C179" s="1" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="F179" s="1" t="n">
         <v>30</v>
@@ -2514,7 +2524,10 @@
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C180" s="1" t="s">
-        <v>43</v>
+        <v>77</v>
+      </c>
+      <c r="F180" s="1" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2524,55 +2537,52 @@
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C182" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F182" s="1" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C183" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F183" s="1" t="n">
         <v>35</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C183" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D183" s="3"/>
-    </row>
     <row r="184" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C184" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D184" s="3"/>
-    </row>
-    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C185" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="1" t="s">
+      <c r="C184" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D184" s="4"/>
+    </row>
+    <row r="185" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C185" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D185" s="4"/>
+    </row>
+    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C186" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B187" s="1" t="s">
+    </row>
+    <row r="188" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C187" s="3" t="s">
+      <c r="B188" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C188" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D187" s="3"/>
-    </row>
-    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C188" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F188" s="1" t="n">
-        <v>70</v>
-      </c>
+      <c r="D188" s="4"/>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C189" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F189" s="1" t="n">
         <v>70</v>
@@ -2580,34 +2590,37 @@
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C190" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F190" s="1" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C191" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D191" s="4"/>
+      <c r="C191" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F191" s="1" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C192" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F192" s="1" t="n">
-        <v>30</v>
-      </c>
+      <c r="C192" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D192" s="5"/>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C193" s="1" t="s">
-        <v>74</v>
+        <v>15</v>
+      </c>
+      <c r="F193" s="1" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C194" s="1" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2617,23 +2630,23 @@
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C196" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E196" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F196" s="1" t="n">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C197" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="E197" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F197" s="1" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C198" s="1" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2643,68 +2656,68 @@
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C200" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G200" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B202" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C201" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G201" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C202" s="3" t="s">
+      <c r="B203" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C203" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D202" s="3"/>
-    </row>
-    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C203" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F203" s="1" t="n">
-        <v>70</v>
-      </c>
+      <c r="D203" s="4"/>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C204" s="1" t="s">
-        <v>15</v>
+        <v>142</v>
       </c>
       <c r="F204" s="1" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C205" s="1" t="s">
-        <v>142</v>
+        <v>15</v>
+      </c>
+      <c r="F205" s="1" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C206" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E206" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F206" s="1" t="n">
-        <v>35</v>
-      </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C207" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="E207" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F207" s="1" t="n">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C208" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="F208" s="1" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C209" s="1" t="s">
@@ -2721,31 +2734,28 @@
         <v>148</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="1" t="s">
+    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C212" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B213" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C213" s="1" t="s">
+      <c r="B214" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C214" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C214" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F214" s="1" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C215" s="1" t="s">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="F215" s="1" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2761,29 +2771,29 @@
         <v>152</v>
       </c>
       <c r="F217" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C218" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F218" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="G217" s="1" t="n">
+      <c r="G218" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C219" s="1" t="s">
+    <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F219" s="1" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C220" s="1" t="s">
         <v>155</v>
       </c>
       <c r="F220" s="1" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2794,9 +2804,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="1" t="s">
+    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C222" s="1" t="s">
         <v>157</v>
+      </c>
+      <c r="F222" s="1" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2815,82 +2828,87 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="2" t="s">
+      <c r="A227" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B227" s="2" t="s">
+    </row>
+    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="5" t="s">
+      <c r="B228" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B228" s="5" t="s">
+    </row>
+    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E228" s="6" t="s">
+      <c r="B229" s="6" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="5" t="s">
+      <c r="E229" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B229" s="5" t="s">
+    </row>
+    <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="E229" s="6" t="s">
+      <c r="B230" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="5" t="s">
+      <c r="E230" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B230" s="5" t="s">
+    </row>
+    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="E230" s="6" t="s">
+      <c r="B231" s="6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="5" t="s">
+      <c r="E231" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B231" s="5" t="s">
+    </row>
+    <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E231" s="6" t="s">
+      <c r="B232" s="6" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="5" t="s">
+      <c r="E232" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B232" s="5" t="s">
+    </row>
+    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="E232" s="6" t="s">
+      <c r="B233" s="6" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="5" t="s">
+      <c r="E233" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B233" s="5" t="s">
+    </row>
+    <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="E233" s="6" t="s">
+      <c r="B234" s="6" t="s">
         <v>180</v>
+      </c>
+      <c r="E234" s="7" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E7:E220" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E7:E221" type="list">
       <formula1>Datatypes!$A$2:$A$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2913,7 +2931,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C72:G72 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2939,12 +2957,12 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2966,7 +2984,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C72:G72 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2992,10 +3010,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>10</v>
@@ -3003,7 +3021,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>30</v>
@@ -3011,7 +3029,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>70</v>
@@ -3019,7 +3037,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>30</v>
@@ -3044,7 +3062,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C72:G72 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3070,10 +3088,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>30</v>
@@ -3081,7 +3099,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>10</v>
@@ -3089,7 +3107,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>30</v>
@@ -3097,7 +3115,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>70</v>
@@ -3105,7 +3123,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>30</v>
@@ -3130,7 +3148,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C72:G72 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3156,7 +3174,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>50</v>
@@ -3167,7 +3185,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>3</v>
@@ -3175,10 +3193,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>35</v>
@@ -3186,7 +3204,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>5000</v>
@@ -3211,7 +3229,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C72:G72 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3237,12 +3255,12 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3264,7 +3282,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="C72:G72 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3290,10 +3308,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>10</v>
@@ -3301,7 +3319,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>10</v>
@@ -3309,7 +3327,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>30</v>
@@ -3317,7 +3335,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>70</v>
@@ -3325,7 +3343,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>30</v>
@@ -3350,7 +3368,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C72:G72 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3376,7 +3394,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
@@ -3387,7 +3405,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>500</v>
@@ -3395,7 +3413,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2</v>
@@ -3403,7 +3421,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>100</v>
@@ -3411,15 +3429,15 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>10</v>
@@ -3427,67 +3445,67 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3509,7 +3527,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C72:G72 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3535,10 +3553,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>35</v>
@@ -3549,22 +3567,22 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -3575,7 +3593,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
@@ -3586,10 +3604,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>10</v>
@@ -3597,10 +3615,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>10</v>
@@ -3608,7 +3626,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>20</v>
@@ -3616,7 +3634,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
@@ -3627,7 +3645,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
@@ -3638,10 +3656,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>10</v>
@@ -3649,10 +3667,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>10</v>
@@ -3660,7 +3678,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>20</v>
@@ -3668,7 +3686,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>10</v>
@@ -3679,10 +3697,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>35</v>
@@ -3693,7 +3711,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>20</v>
@@ -3704,7 +3722,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
@@ -3715,7 +3733,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3737,7 +3755,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="C72:G72 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3746,24 +3764,24 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>250</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3773,7 +3791,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3783,12 +3801,12 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3810,7 +3828,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C72:G72 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3837,7 +3855,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>70</v>
@@ -3845,7 +3863,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>30</v>
@@ -3853,10 +3871,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>49</v>
+        <v>184</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>35</v>
@@ -3864,7 +3882,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>100</v>
@@ -3872,7 +3890,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2</v>
@@ -3903,7 +3921,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="C72:G72 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3929,7 +3947,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>50</v>
@@ -3937,12 +3955,12 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>70</v>
@@ -3950,7 +3968,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>70</v>
@@ -3958,7 +3976,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3980,7 +3998,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C72:G72 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4006,7 +4024,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>70</v>
@@ -4014,7 +4032,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>30</v>
@@ -4022,7 +4040,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>30</v>
@@ -4030,12 +4048,12 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>70</v>
@@ -4043,7 +4061,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>30</v>
@@ -4051,7 +4069,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>100</v>
@@ -4076,7 +4094,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C72:G72 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4102,7 +4120,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>3</v>
@@ -4110,7 +4128,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>500</v>
@@ -4135,7 +4153,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="C72:G72 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4161,7 +4179,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>70</v>
@@ -4169,7 +4187,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>50</v>
@@ -4177,7 +4195,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>30</v>
@@ -4185,7 +4203,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>100</v>
@@ -4210,7 +4228,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C72:G72 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4236,10 +4254,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>35</v>
@@ -4247,10 +4265,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>35</v>
@@ -4275,7 +4293,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C72:G72 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4301,7 +4319,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>250</v>
@@ -4309,7 +4327,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>50</v>
@@ -4317,7 +4335,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>30</v>
@@ -4345,7 +4363,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C72:G72 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4371,10 +4389,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>10</v>
@@ -4382,7 +4400,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>3</v>
@@ -4390,7 +4408,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>30</v>
@@ -4398,7 +4416,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>70</v>
@@ -4406,7 +4424,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>30</v>

</xml_diff>

<commit_message>
Add in patient table column pat.name.use in
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="table_description_collapsed" sheetId="1" state="visible" r:id="rId3"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="255">
   <si>
     <t xml:space="preserve">RESOURCE</t>
   </si>
@@ -643,6 +643,9 @@
   </si>
   <si>
     <t xml:space="preserve">end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use</t>
   </si>
   <si>
     <t xml:space="preserve">family</t>
@@ -911,7 +914,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -922,10 +925,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1200,8 +1199,8 @@
   </sheetPr>
   <dimension ref="A1:G234"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2038,10 +2037,10 @@
       <c r="B114" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="C114" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D114" s="4"/>
+      <c r="D114" s="3"/>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="1" t="s">
@@ -2068,10 +2067,10 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="5" t="s">
+      <c r="C118" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D118" s="5"/>
+      <c r="D118" s="4"/>
       <c r="G118" s="1" t="n">
         <v>2</v>
       </c>
@@ -2127,10 +2126,10 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C126" s="4" t="s">
+      <c r="C126" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D126" s="4"/>
+      <c r="D126" s="3"/>
       <c r="E126" s="1" t="s">
         <v>38</v>
       </c>
@@ -2139,16 +2138,16 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="4" t="s">
+      <c r="C127" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D127" s="4"/>
+      <c r="D127" s="3"/>
     </row>
     <row r="128" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C128" s="4" t="s">
+      <c r="C128" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D128" s="4"/>
+      <c r="D128" s="3"/>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="1" t="s">
@@ -2186,10 +2185,10 @@
       <c r="B134" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="C134" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D134" s="4"/>
+      <c r="D134" s="3"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="1" t="s">
@@ -2216,10 +2215,10 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C138" s="5" t="s">
+      <c r="C138" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D138" s="5"/>
+      <c r="D138" s="4"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="1" t="s">
@@ -2309,10 +2308,10 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="4" t="s">
+      <c r="C151" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D151" s="4"/>
+      <c r="D151" s="3"/>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="1" t="s">
@@ -2374,10 +2373,10 @@
       <c r="B160" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C160" s="4" t="s">
+      <c r="C160" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D160" s="4"/>
+      <c r="D160" s="3"/>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C161" s="1" t="s">
@@ -2436,8 +2435,8 @@
       <c r="C168" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F168" s="4"/>
-      <c r="G168" s="4"/>
+      <c r="F168" s="3"/>
+      <c r="G168" s="3"/>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C169" s="1" t="s">
@@ -2462,10 +2461,10 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C171" s="4" t="s">
+      <c r="C171" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D171" s="4"/>
+      <c r="D171" s="3"/>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C172" s="1" t="s">
@@ -2487,10 +2486,10 @@
       <c r="B175" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C175" s="4" t="s">
+      <c r="C175" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D175" s="4"/>
+      <c r="D175" s="3"/>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C176" s="1" t="s">
@@ -2509,10 +2508,10 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="5" t="s">
+      <c r="C178" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D178" s="5"/>
+      <c r="D178" s="4"/>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C179" s="1" t="s">
@@ -2552,16 +2551,16 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C184" s="4" t="s">
+      <c r="C184" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D184" s="4"/>
+      <c r="D184" s="3"/>
     </row>
     <row r="185" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C185" s="4" t="s">
+      <c r="C185" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D185" s="4"/>
+      <c r="D185" s="3"/>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C186" s="1" t="s">
@@ -2575,10 +2574,10 @@
       <c r="B188" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C188" s="4" t="s">
+      <c r="C188" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D188" s="4"/>
+      <c r="D188" s="3"/>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C189" s="1" t="s">
@@ -2605,10 +2604,10 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C192" s="5" t="s">
+      <c r="C192" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D192" s="5"/>
+      <c r="D192" s="4"/>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C193" s="1" t="s">
@@ -2674,10 +2673,10 @@
       <c r="B203" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C203" s="4" t="s">
+      <c r="C203" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D203" s="4"/>
+      <c r="D203" s="3"/>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C204" s="1" t="s">
@@ -2841,68 +2840,68 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="6" t="s">
+      <c r="A229" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B229" s="6" t="s">
+      <c r="B229" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E229" s="7" t="s">
+      <c r="E229" s="6" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="6" t="s">
+      <c r="A230" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B230" s="6" t="s">
+      <c r="B230" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E230" s="7" t="s">
+      <c r="E230" s="6" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="6" t="s">
+      <c r="A231" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B231" s="6" t="s">
+      <c r="B231" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="E231" s="7" t="s">
+      <c r="E231" s="6" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="6" t="s">
+      <c r="A232" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B232" s="6" t="s">
+      <c r="B232" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="E232" s="7" t="s">
+      <c r="E232" s="6" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="6" t="s">
+      <c r="A233" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B233" s="6" t="s">
+      <c r="B233" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="E233" s="7" t="s">
+      <c r="E233" s="6" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="6" t="s">
+      <c r="A234" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B234" s="6" t="s">
+      <c r="B234" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="E234" s="7" t="s">
+      <c r="E234" s="6" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2957,12 +2956,12 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3010,10 +3009,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>10</v>
@@ -3021,7 +3020,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>30</v>
@@ -3088,10 +3087,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>30</v>
@@ -3099,7 +3098,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>10</v>
@@ -3107,7 +3106,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>30</v>
@@ -3174,7 +3173,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>50</v>
@@ -3185,7 +3184,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>3</v>
@@ -3193,7 +3192,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>38</v>
@@ -3255,12 +3254,12 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3308,10 +3307,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>10</v>
@@ -3319,7 +3318,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>10</v>
@@ -3327,7 +3326,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>30</v>
@@ -3394,7 +3393,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
@@ -3413,7 +3412,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>2</v>
@@ -3421,7 +3420,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>100</v>
@@ -3429,12 +3428,12 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>71</v>
@@ -3445,17 +3444,17 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3465,47 +3464,47 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3553,7 +3552,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>38</v>
@@ -3567,22 +3566,22 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -3593,7 +3592,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
@@ -3604,10 +3603,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>10</v>
@@ -3615,10 +3614,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>10</v>
@@ -3626,7 +3625,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>20</v>
@@ -3634,7 +3633,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
@@ -3645,7 +3644,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
@@ -3656,10 +3655,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>10</v>
@@ -3667,10 +3666,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>10</v>
@@ -3678,7 +3677,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>20</v>
@@ -3686,7 +3685,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>10</v>
@@ -3697,10 +3696,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>35</v>
@@ -3711,7 +3710,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>20</v>
@@ -3722,7 +3721,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
@@ -3764,19 +3763,19 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="7" t="s">
         <v>251</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3791,7 +3790,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3806,7 +3805,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3873,7 +3872,7 @@
       <c r="A4" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="1" t="n">
@@ -4290,10 +4289,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4318,19 +4317,20 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>250</v>
+      <c r="A2" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>50</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4338,9 +4338,17 @@
         <v>203</v>
       </c>
       <c r="C4" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D5" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -4389,10 +4397,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>10</v>
@@ -4400,7 +4408,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>3</v>
@@ -4408,7 +4416,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>30</v>

</xml_diff>

<commit_message>
Add calculated_ref columns in TableDescription and DB
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -12,21 +12,22 @@
     <sheet name="Id" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Identifier" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Reference" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="CodeableConcept" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="Coding" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="Period" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="HumanName" sheetId="8" state="visible" r:id="rId10"/>
-    <sheet name="Age" sheetId="9" state="visible" r:id="rId11"/>
-    <sheet name="Range" sheetId="10" state="visible" r:id="rId12"/>
-    <sheet name="SimpleQuantity" sheetId="11" state="visible" r:id="rId13"/>
-    <sheet name="Duration" sheetId="12" state="visible" r:id="rId14"/>
-    <sheet name="Annotation" sheetId="13" state="visible" r:id="rId15"/>
-    <sheet name="Ratio" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="Quantity" sheetId="15" state="visible" r:id="rId17"/>
-    <sheet name="Dosage" sheetId="16" state="visible" r:id="rId18"/>
-    <sheet name="Timing" sheetId="17" state="visible" r:id="rId19"/>
-    <sheet name="Provision" sheetId="18" state="visible" r:id="rId20"/>
-    <sheet name="Datatypes" sheetId="19" state="visible" r:id="rId21"/>
+    <sheet name="CalculatedReference" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="CodeableConcept" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="Coding" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="Period" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="HumanName" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="Age" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="Range" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="SimpleQuantity" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="Duration" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet name="Annotation" sheetId="14" state="visible" r:id="rId16"/>
+    <sheet name="Ratio" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="Quantity" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="Dosage" sheetId="17" state="visible" r:id="rId19"/>
+    <sheet name="Timing" sheetId="18" state="visible" r:id="rId20"/>
+    <sheet name="Provision" sheetId="19" state="visible" r:id="rId21"/>
+    <sheet name="Datatypes" sheetId="20" state="visible" r:id="rId22"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="259">
   <si>
     <t xml:space="preserve">RESOURCE</t>
   </si>
@@ -82,243 +83,246 @@
     <t xml:space="preserve">subject/reference</t>
   </si>
   <si>
+    <t xml:space="preserve">partOf/CalculatedReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">class/Coding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serviceType/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">period/Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnosis/condition/CalculatedReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnosis/use/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnosis/rank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hospitalization/admitSource/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hospitalization/dischargeDisposition/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location/location/Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location/status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location/physicalType/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serviceProvider/Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name/HumanName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birthDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deceasedDateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address/postalCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">con</t>
+  </si>
+  <si>
+    <t xml:space="preserve">encounter/CalculatedReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clinicalStatus/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verificationStatus/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">severity/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bodySite/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onsetPeriod/Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onsetDateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abatementDateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abatementAge/Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abatementPeriod/Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abatementRange/Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abatementString</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recordedDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recorder/Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asserter/Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stage/summary/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stage/assessment/Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stage/type/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note/Annotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">med</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount/Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingredient/strength/Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingredient/itemCodeableConcept/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingredient/itemReference/Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingredient/isActive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationRequest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medreq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medicationReference/reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">statusReason/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">priority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reportedBoolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reportedReference/Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medicationCodeableConcept/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supportingInformation/Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">authoredOn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">requester/Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonCode/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonReference/Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">basedOn/Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dosageInstruction/Dosage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">substitution/reason/CodeableConcept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MedicationAdministration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medadm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">context/CalculatedReference</t>
+  </si>
+  <si>
     <t xml:space="preserve">partOf/reference</t>
   </si>
   <si>
-    <t xml:space="preserve">status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class/Coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serviceType/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">period/Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnosis/condition/reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnosis/use/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnosis/rank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hospitalization/admitSource/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hospitalization/dischargeDisposition/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location/location/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location/status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location/physicalType/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serviceProvider/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name/HumanName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birthDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deceasedDateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">address/postalCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">con</t>
-  </si>
-  <si>
-    <t xml:space="preserve">encounter/reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clinicalStatus/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verificationStatus/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">severity/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">code/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bodySite/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">onsetPeriod/Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">onsetDateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abatementDateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abatementAge/Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abatementPeriod/Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abatementRange/Range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abatementString</t>
-  </si>
-  <si>
-    <t xml:space="preserve">recordedDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">recorder/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asserter/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stage/summary/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stage/assessment/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stage/type/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">note/Annotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">med</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amount/Ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ingredient/strength/Ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ingredient/itemCodeableConcept/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ingredient/itemReference/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ingredient/isActive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MedicationRequest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medreq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medicationReference/reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">statusReason/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">priority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reportedBoolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reportedReference/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medicationCodeableConcept/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supportingInformation/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">authoredOn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">requester/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasonCode/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasonReference/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">basedOn/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dosageInstruction/Dosage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">substitution/reason/CodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MedicationAdministration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medadm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">context/reference</t>
-  </si>
-  <si>
     <t xml:space="preserve">effectiveDateTime</t>
   </si>
   <si>
@@ -617,6 +621,12 @@
   </si>
   <si>
     <t xml:space="preserve">display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculated_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Note: this is not a FHIR column and will be always empty in FHIR data but it will create the column in the database</t>
   </si>
   <si>
     <t xml:space="preserve">coding/Coding</t>
@@ -932,6 +942,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -940,10 +954,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1203,19 +1213,19 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A191" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C216" activeCellId="0" sqref="C216"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.85"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1242,54 +1252,76 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="1" t="s">
@@ -1318,10 +1350,10 @@
       <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="3" t="n">
         <v>70</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="G15" s="3" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1340,10 +1372,10 @@
       <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="1" t="n">
+      <c r="F17" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G17" s="1" t="n">
+      <c r="G17" s="3" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1372,10 +1404,10 @@
       <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="1" t="n">
+      <c r="F21" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="G21" s="1" t="n">
+      <c r="G21" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1393,15 +1425,16 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="1" t="s">
@@ -1415,9 +1448,10 @@
       <c r="C27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="1" t="n">
+      <c r="F27" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="1" t="s">
@@ -1426,58 +1460,63 @@
       <c r="E28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="1" t="n">
+      <c r="F28" s="3" t="n">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="3" t="s">
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="1" t="n">
+      <c r="F29" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="1" t="n">
+      <c r="F30" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="G30" s="1" t="n">
+      <c r="G30" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F33" s="1" t="n">
+      <c r="F33" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F34" s="1" t="n">
+      <c r="F34" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
@@ -1527,9 +1566,10 @@
       <c r="E42" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="1" t="n">
+      <c r="F42" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="1" t="s">
@@ -1538,9 +1578,10 @@
       <c r="E43" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F43" s="1" t="n">
+      <c r="F43" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1" t="s">
@@ -1561,9 +1602,10 @@
       <c r="C47" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F47" s="1" t="n">
+      <c r="F47" s="3" t="n">
         <v>300</v>
       </c>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1" t="s">
@@ -1572,9 +1614,10 @@
       <c r="E48" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F48" s="1" t="n">
+      <c r="F48" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="s">
@@ -1619,15 +1662,16 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="1" t="s">
@@ -1641,9 +1685,10 @@
       <c r="C58" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F58" s="1" t="n">
+      <c r="F58" s="3" t="n">
         <v>20</v>
       </c>
+      <c r="G58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="1" t="s">
@@ -1686,39 +1731,42 @@
       <c r="E64" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F64" s="1" t="n">
+      <c r="F64" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="G64" s="1" t="n">
+      <c r="G64" s="3" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F67" s="1" t="n">
+      <c r="F67" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F68" s="1" t="n">
+      <c r="F68" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="1" t="s">
@@ -1727,17 +1775,19 @@
       <c r="D69" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F69" s="1" t="n">
+      <c r="F69" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F70" s="1" t="n">
+      <c r="F70" s="3" t="n">
         <v>20</v>
       </c>
+      <c r="G70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="1" t="s">
@@ -1748,17 +1798,19 @@
       <c r="C72" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F72" s="1" t="n">
+      <c r="F72" s="3" t="n">
         <v>20</v>
       </c>
+      <c r="G72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F73" s="1" t="n">
+      <c r="F73" s="3" t="n">
         <v>20</v>
       </c>
+      <c r="G73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="1" t="s">
@@ -1772,9 +1824,10 @@
       <c r="C75" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F75" s="1" t="n">
+      <c r="F75" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="G75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="1" t="s">
@@ -1783,9 +1836,10 @@
       <c r="E76" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F76" s="1" t="n">
+      <c r="F76" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="G76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="1" t="s">
@@ -1812,9 +1866,10 @@
       <c r="E80" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F80" s="1" t="n">
+      <c r="F80" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="1" t="s">
@@ -1867,47 +1922,52 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D89" s="3"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F90" s="1" t="n">
+      <c r="F90" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F91" s="1" t="n">
+      <c r="F91" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F92" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="F92" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F93" s="1" t="n">
+      <c r="F93" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="G93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="1" t="s">
@@ -1926,9 +1986,10 @@
       <c r="D96" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F96" s="1" t="n">
+      <c r="F96" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G96" s="3"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="1" t="s">
@@ -1945,23 +2006,24 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F99" s="1" t="n">
+      <c r="F99" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G99" s="3"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,11 +2044,12 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F104" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="F104" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="1" t="s">
@@ -1998,83 +2061,87 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F106" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="F106" s="3" t="n">
         <v>100</v>
       </c>
+      <c r="G106" s="3"/>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B114" s="1" t="s">
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="B114" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C114" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D114" s="3"/>
+      <c r="D114" s="4"/>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F115" s="1" t="n">
+      <c r="F115" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G115" s="3"/>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F116" s="1" t="n">
+      <c r="F116" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G116" s="3"/>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C117" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F117" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="F117" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G117" s="3"/>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="4" t="s">
+      <c r="C118" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D118" s="4"/>
+      <c r="D118" s="5"/>
       <c r="G118" s="1" t="n">
         <v>2</v>
       </c>
@@ -2083,9 +2150,10 @@
       <c r="C119" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F119" s="1" t="n">
+      <c r="F119" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="G119" s="3"/>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C120" s="1" t="s">
@@ -2104,9 +2172,10 @@
       <c r="D122" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F122" s="1" t="n">
+      <c r="F122" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G122" s="3"/>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="1" t="s">
@@ -2115,43 +2184,45 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F124" s="1" t="n">
+      <c r="F124" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G124" s="3"/>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C125" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C126" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D126" s="3"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C126" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D126" s="4"/>
       <c r="E126" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F126" s="1" t="n">
+      <c r="F126" s="3" t="n">
         <v>35</v>
       </c>
-    </row>
-    <row r="127" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D127" s="3"/>
-    </row>
-    <row r="128" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C128" s="3" t="s">
+      <c r="G126" s="3"/>
+    </row>
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C127" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D128" s="3"/>
+      <c r="D127" s="4"/>
+    </row>
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C128" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D128" s="4"/>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="1" t="s">
@@ -2176,61 +2247,65 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C132" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G132" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B134" s="1" t="s">
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C134" s="3" t="s">
+      <c r="B134" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C134" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D134" s="3"/>
+      <c r="D134" s="4"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F135" s="1" t="n">
+      <c r="F135" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G135" s="3"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F136" s="1" t="n">
+      <c r="F136" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F137" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="F137" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G137" s="3"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C138" s="4" t="s">
+      <c r="C138" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D138" s="4"/>
+      <c r="D138" s="5"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F139" s="1" t="n">
+      <c r="F139" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="G139" s="3"/>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="1" t="s">
@@ -2244,29 +2319,31 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F142" s="1" t="n">
+      <c r="F142" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G142" s="3"/>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C143" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F143" s="1" t="n">
+      <c r="F143" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G143" s="3"/>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C144" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G144" s="1" t="n">
         <v>2</v>
@@ -2274,7 +2351,7 @@
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C145" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G145" s="1" t="n">
         <v>2</v>
@@ -2282,7 +2359,7 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G146" s="1" t="n">
         <v>2</v>
@@ -2290,7 +2367,7 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C147" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G147" s="1" t="n">
         <v>2</v>
@@ -2298,7 +2375,7 @@
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,18 +2385,18 @@
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D151" s="3"/>
+    </row>
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C151" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D151" s="4"/>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G152" s="1" t="n">
         <v>3</v>
@@ -2327,7 +2404,7 @@
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C153" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G153" s="1" t="n">
         <v>3</v>
@@ -2335,7 +2412,7 @@
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C154" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G154" s="1" t="n">
         <v>3</v>
@@ -2343,7 +2420,7 @@
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C155" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G155" s="1" t="n">
         <v>3</v>
@@ -2351,7 +2428,7 @@
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C156" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G156" s="1" t="n">
         <v>3</v>
@@ -2359,76 +2436,83 @@
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F157" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="F157" s="3" t="n">
         <v>500</v>
       </c>
+      <c r="G157" s="3"/>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B160" s="1" t="s">
+    </row>
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C160" s="3" t="s">
+      <c r="B160" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C160" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D160" s="3"/>
+      <c r="D160" s="4"/>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C161" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F161" s="1" t="n">
+      <c r="F161" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G161" s="3"/>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C162" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F162" s="1" t="n">
+      <c r="F162" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G162" s="3"/>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C163" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F163" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="F163" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G163" s="3"/>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C164" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F164" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="F164" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G164" s="3"/>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C165" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F165" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="F165" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G165" s="3"/>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F166" s="1" t="n">
+      <c r="F166" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="G166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C167" s="1" t="s">
@@ -2439,99 +2523,106 @@
       <c r="C168" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F168" s="3"/>
-      <c r="G168" s="3"/>
+      <c r="F168" s="4"/>
+      <c r="G168" s="4"/>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C169" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F169" s="1" t="n">
+      <c r="F169" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G169" s="3"/>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C170" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F170" s="1" t="n">
+      <c r="F170" s="3" t="n">
         <v>35</v>
       </c>
-    </row>
-    <row r="171" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C171" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D171" s="3"/>
+      <c r="G170" s="3"/>
+    </row>
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C171" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D171" s="4"/>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C172" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F172" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="F172" s="3" t="n">
         <v>500</v>
       </c>
+      <c r="G172" s="3"/>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C173" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B175" s="1" t="s">
+    </row>
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C175" s="3" t="s">
+      <c r="B175" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C175" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D175" s="3"/>
+      <c r="D175" s="4"/>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C176" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F176" s="1" t="n">
+      <c r="F176" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G176" s="3"/>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C177" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F177" s="1" t="n">
+      <c r="F177" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G177" s="3"/>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="4" t="s">
+      <c r="C178" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D178" s="4"/>
+      <c r="D178" s="5"/>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C179" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F179" s="1" t="n">
+      <c r="F179" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="G179" s="3"/>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C180" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F180" s="1" t="n">
+      <c r="F180" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="G180" s="3"/>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C181" s="1" t="s">
@@ -2550,76 +2641,81 @@
       <c r="E183" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F183" s="1" t="n">
+      <c r="F183" s="3" t="n">
         <v>35</v>
       </c>
-    </row>
-    <row r="184" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C184" s="3" t="s">
+      <c r="G183" s="3"/>
+    </row>
+    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C184" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D184" s="3"/>
-    </row>
-    <row r="185" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C185" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D185" s="3"/>
+      <c r="D184" s="4"/>
+    </row>
+    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C185" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D185" s="4"/>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C186" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B188" s="1" t="s">
+    </row>
+    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C188" s="3" t="s">
+      <c r="B188" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C188" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D188" s="3"/>
+      <c r="D188" s="4"/>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C189" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F189" s="1" t="n">
+      <c r="F189" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G189" s="3"/>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C190" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F190" s="1" t="n">
+      <c r="F190" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G190" s="3"/>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C191" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F191" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="F191" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G191" s="3"/>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C192" s="4" t="s">
+      <c r="C192" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D192" s="4"/>
+      <c r="D192" s="5"/>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C193" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F193" s="1" t="n">
+      <c r="F193" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="G193" s="3"/>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C194" s="1" t="s">
@@ -2638,18 +2734,19 @@
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C197" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F197" s="1" t="n">
+      <c r="F197" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G197" s="3"/>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C198" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2670,230 +2767,265 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B203" s="1" t="s">
+    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C203" s="3" t="s">
+      <c r="B203" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C203" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D203" s="3"/>
+      <c r="D203" s="4"/>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C204" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F204" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="F204" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G204" s="3"/>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C205" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F205" s="1" t="n">
+      <c r="F205" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="G205" s="3"/>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C206" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C207" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F207" s="1" t="n">
+      <c r="F207" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="G207" s="3"/>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C208" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C209" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="1" t="s">
+      <c r="A211" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B211" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C211" s="1" t="s">
+      <c r="B211" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C211" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D211" s="3"/>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C212" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F212" s="1" t="n">
+      <c r="F212" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="G212" s="3"/>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C213" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F213" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="F213" s="3" t="n">
         <v>50</v>
       </c>
+      <c r="G213" s="3"/>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C214" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F214" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="F214" s="3" t="n">
         <v>50</v>
       </c>
+      <c r="G214" s="3"/>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C215" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F215" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="F215" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G215" s="1" t="n">
+      <c r="G215" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C216" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C218" s="1" t="s">
+      <c r="A218" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F218" s="1" t="n">
+      <c r="B218" s="3"/>
+      <c r="C218" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D218" s="3"/>
+      <c r="F218" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="G218" s="3"/>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C219" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F219" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="F219" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="G219" s="3"/>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C220" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F220" s="1" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="1" t="s">
-        <v>156</v>
-      </c>
+      <c r="A222" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B222" s="3"/>
+      <c r="C222" s="3"/>
+      <c r="D222" s="3"/>
+      <c r="E222" s="3"/>
+      <c r="F222" s="3"/>
+      <c r="G222" s="3"/>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="1" t="s">
-        <v>157</v>
-      </c>
+      <c r="A223" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B223" s="3"/>
+      <c r="C223" s="3"/>
+      <c r="D223" s="3"/>
+      <c r="E223" s="3"/>
+      <c r="F223" s="3"/>
+      <c r="G223" s="3"/>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="A224" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B224" s="3"/>
+      <c r="C224" s="3"/>
+      <c r="D224" s="3"/>
+      <c r="E224" s="3"/>
+      <c r="F224" s="3"/>
+      <c r="G224" s="3"/>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="1" t="s">
-        <v>159</v>
-      </c>
+      <c r="A225" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B225" s="3"/>
+      <c r="C225" s="3"/>
+      <c r="D225" s="3"/>
+      <c r="E225" s="3"/>
+      <c r="F225" s="3"/>
+      <c r="G225" s="3"/>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B227" s="5" t="s">
+      <c r="A227" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="E227" s="6" t="s">
+      <c r="B227" s="6" t="s">
         <v>164</v>
       </c>
+      <c r="E227" s="3" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B228" s="5" t="s">
+      <c r="A228" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="E228" s="6" t="s">
+      <c r="B228" s="6" t="s">
         <v>167</v>
       </c>
+      <c r="E228" s="3" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B229" s="5" t="s">
+      <c r="A229" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E229" s="6" t="s">
+      <c r="B229" s="6" t="s">
         <v>170</v>
       </c>
+      <c r="E229" s="3" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B230" s="5" t="s">
+      <c r="A230" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E230" s="6" t="s">
+      <c r="B230" s="6" t="s">
         <v>173</v>
       </c>
+      <c r="E230" s="3" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B231" s="5" t="s">
+      <c r="A231" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E231" s="6" t="s">
+      <c r="B231" s="6" t="s">
         <v>176</v>
       </c>
+      <c r="E231" s="3" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B232" s="5" t="s">
+      <c r="A232" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="E232" s="6" t="s">
+      <c r="B232" s="6" t="s">
         <v>179</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2925,15 +3057,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
   </cols>
@@ -2953,13 +3085,50 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>207</v>
       </c>
+      <c r="C2" s="3" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>208</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2978,15 +3147,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
   </cols>
@@ -3006,39 +3175,18 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>10</v>
-      </c>
+      <c r="A2" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>30</v>
-      </c>
+      <c r="A3" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3056,13 +3204,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -3084,45 +3232,40 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="A2" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>30</v>
+      <c r="A4" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" s="1" t="n">
+      <c r="A5" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="n">
         <v>30</v>
       </c>
     </row>
@@ -3142,15 +3285,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
   </cols>
@@ -3170,41 +3313,50 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>35</v>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>5000</v>
+      <c r="A5" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3223,15 +3375,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
   </cols>
@@ -3251,13 +3403,45 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>212</v>
       </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>213</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="n">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
@@ -3276,15 +3460,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
   </cols>
@@ -3304,47 +3488,18 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>10</v>
-      </c>
+      <c r="A2" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>30</v>
-      </c>
+      <c r="A3" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3362,17 +3517,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="43.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3390,119 +3545,46 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="A2" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>500</v>
+      <c r="A3" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>100</v>
+      <c r="A5" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>230</v>
+      <c r="A6" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3523,15 +3605,15 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="43.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3549,188 +3631,119 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3749,17 +3762,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3777,59 +3790,190 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="A2" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="B17" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="C18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3846,63 +3990,87 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B1" s="6" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3921,11 +4089,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -3948,45 +4116,54 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="A2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C3" s="1" t="n">
+      <c r="A3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" s="1" t="n">
+      <c r="A5" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="n">
         <v>100</v>
       </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D6" s="1" t="n">
+      <c r="A6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="n">
         <v>2</v>
       </c>
     </row>
@@ -4001,8 +4178,81 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;KffffffSeite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffSeite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.86"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -4014,11 +4264,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4040,38 +4290,45 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="A2" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>186</v>
-      </c>
+      <c r="A3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4" s="1" t="n">
+      <c r="A4" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5" s="1" t="n">
+      <c r="A5" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>189</v>
-      </c>
+      <c r="A6" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4091,11 +4348,11 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4117,55 +4374,63 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="A2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" s="1" t="n">
+      <c r="A3" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C4" s="1" t="n">
+      <c r="A4" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>186</v>
-      </c>
+      <c r="A5" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C6" s="1" t="n">
+      <c r="A6" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C7" s="1" t="n">
+      <c r="A7" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C8" s="1" t="n">
+      <c r="A8" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="n">
         <v>100</v>
       </c>
     </row>
@@ -4185,13 +4450,100 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.44"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4213,94 +4565,22 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D2" s="1" t="n">
+      <c r="A2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" s="1" t="n">
+      <c r="A3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="n">
         <v>500</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4319,15 +4599,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
   </cols>
@@ -4347,25 +4627,39 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>35</v>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>35</v>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4384,13 +4678,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4412,38 +4706,25 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>30</v>
+      <c r="A2" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>10</v>
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -4462,13 +4743,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4490,46 +4771,42 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3" t="n">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new table description version with fixed column names
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="262">
   <si>
     <t xml:space="preserve">RESOURCE</t>
   </si>
@@ -564,6 +564,15 @@
   </si>
   <si>
     <t xml:space="preserve"># replace 'context_reference' by 'encounter_ref' in column names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_context_calculated_ref$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_encounter_calculated_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># replace 'context_calculated_ref' by 'encounter_calculated_ref' in column names</t>
   </si>
   <si>
     <t xml:space="preserve">_reference$</t>
@@ -1213,11 +1222,11 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A211" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E231" activeCellId="0" sqref="E231"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.86"/>
@@ -1465,7 +1474,7 @@
       </c>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="4" t="s">
         <v>37</v>
       </c>
@@ -2098,7 +2107,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
         <v>105</v>
       </c>
@@ -2199,7 +2208,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="4" t="s">
         <v>107</v>
       </c>
@@ -2212,13 +2221,13 @@
       </c>
       <c r="G126" s="3"/>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="4" t="s">
         <v>108</v>
       </c>
       <c r="D127" s="4"/>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="4" t="s">
         <v>109</v>
       </c>
@@ -2253,7 +2262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
         <v>111</v>
       </c>
@@ -2388,7 +2397,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C151" s="4" t="s">
         <v>120</v>
       </c>
@@ -2448,7 +2457,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="s">
         <v>128</v>
       </c>
@@ -2550,7 +2559,7 @@
       </c>
       <c r="G170" s="3"/>
     </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C171" s="4" t="s">
         <v>120</v>
       </c>
@@ -2570,7 +2579,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="3" t="s">
         <v>134</v>
       </c>
@@ -2646,13 +2655,13 @@
       </c>
       <c r="G183" s="3"/>
     </row>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C184" s="4" t="s">
         <v>84</v>
       </c>
       <c r="D184" s="4"/>
     </row>
-    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C185" s="4" t="s">
         <v>120</v>
       </c>
@@ -2663,7 +2672,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="3" t="s">
         <v>137</v>
       </c>
@@ -2767,7 +2776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="3" t="s">
         <v>141</v>
       </c>
@@ -3028,7 +3037,17 @@
         <v>180</v>
       </c>
     </row>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B233" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3059,11 +3078,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -3086,10 +3105,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>10</v>
@@ -3097,7 +3116,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="n">
@@ -3106,7 +3125,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="n">
@@ -3115,7 +3134,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="n">
@@ -3124,7 +3143,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="n">
@@ -3149,11 +3168,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -3176,14 +3195,14 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3206,11 +3225,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -3233,10 +3252,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>10</v>
@@ -3244,7 +3263,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="n">
@@ -3253,7 +3272,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="n">
@@ -3262,7 +3281,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="n">
@@ -3287,11 +3306,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -3314,10 +3333,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>30</v>
@@ -3325,7 +3344,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="n">
@@ -3334,7 +3353,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="n">
@@ -3343,7 +3362,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="n">
@@ -3352,7 +3371,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="n">
@@ -3377,11 +3396,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -3404,7 +3423,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="n">
@@ -3416,7 +3435,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3426,7 +3445,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>38</v>
@@ -3437,7 +3456,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="n">
@@ -3462,11 +3481,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -3489,14 +3508,14 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3519,11 +3538,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E231 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
@@ -3546,10 +3565,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>10</v>
@@ -3557,7 +3576,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>10</v>
@@ -3565,7 +3584,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>30</v>
@@ -3573,7 +3592,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>70</v>
@@ -3581,7 +3600,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>30</v>
@@ -3605,11 +3624,11 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="43.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
@@ -3632,7 +3651,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>23</v>
@@ -3643,7 +3662,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>500</v>
@@ -3651,7 +3670,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>2</v>
@@ -3659,7 +3678,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>100</v>
@@ -3667,12 +3686,12 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>71</v>
@@ -3683,17 +3702,17 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3703,47 +3722,47 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3764,11 +3783,11 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
@@ -3791,7 +3810,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>38</v>
@@ -3805,22 +3824,22 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -3831,7 +3850,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>23</v>
@@ -3842,10 +3861,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>10</v>
@@ -3853,10 +3872,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>10</v>
@@ -3864,7 +3883,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>20</v>
@@ -3872,7 +3891,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>23</v>
@@ -3883,7 +3902,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>23</v>
@@ -3894,10 +3913,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>10</v>
@@ -3905,10 +3924,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>10</v>
@@ -3916,7 +3935,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>20</v>
@@ -3924,7 +3943,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>10</v>
@@ -3935,10 +3954,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>35</v>
@@ -3949,7 +3968,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>20</v>
@@ -3960,7 +3979,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>23</v>
@@ -3992,11 +4011,11 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="E231 A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
@@ -4019,7 +4038,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>10</v>
@@ -4033,12 +4052,12 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4048,7 +4067,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4089,11 +4108,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E231 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4117,7 +4136,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="n">
@@ -4127,7 +4146,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="n">
@@ -4137,7 +4156,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>38</v>
@@ -4149,7 +4168,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="n">
@@ -4159,7 +4178,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -4178,8 +4197,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffSeite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;KffffffSeite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4191,29 +4210,29 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="E231 A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4228,7 +4247,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4243,7 +4262,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -4264,11 +4283,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="E231 A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4291,7 +4310,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="n">
@@ -4300,14 +4319,14 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="n">
@@ -4316,7 +4335,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="n">
@@ -4325,7 +4344,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -4348,11 +4367,11 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E231 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4375,7 +4394,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="n">
@@ -4384,7 +4403,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="n">
@@ -4393,7 +4412,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="n">
@@ -4402,14 +4421,14 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="n">
@@ -4418,7 +4437,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="n">
@@ -4427,7 +4446,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="n">
@@ -4452,11 +4471,11 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E231 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.44"/>
   </cols>
@@ -4477,7 +4496,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="n">
@@ -4486,14 +4505,14 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="n">
         <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4526,8 +4545,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4539,11 +4558,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E231 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4566,7 +4585,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4576,7 +4595,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="n">
@@ -4601,11 +4620,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="E231 A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4628,7 +4647,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="n">
@@ -4637,7 +4656,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="n">
@@ -4646,7 +4665,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="n">
@@ -4655,7 +4674,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="n">
@@ -4680,11 +4699,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="E231 C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4707,7 +4726,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>38</v>
@@ -4718,7 +4737,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>38</v>
@@ -4745,11 +4764,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="E231 C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
@@ -4772,7 +4791,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="n">
@@ -4781,7 +4800,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="n">
@@ -4790,7 +4809,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="n">
@@ -4799,7 +4818,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="n">

</xml_diff>

<commit_message>
Add new column for main encounter ref
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="261">
   <si>
     <t xml:space="preserve">RESOURCE</t>
   </si>
@@ -56,12 +56,6 @@
     <t xml:space="preserve">FHIR_TYPE</t>
   </si>
   <si>
-    <t xml:space="preserve">SINGLE_LENGTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNT</t>
-  </si>
-  <si>
     <t xml:space="preserve"># Der Header der Tabelle muss in Zeile 1 stehen. Alle Zeilen, bei denen die Spalte 'FHIR_EXPRESSION'</t>
   </si>
   <si>
@@ -84,6 +78,9 @@
   </si>
   <si>
     <t xml:space="preserve">partOf/CalculatedReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">main/encounter/calculated/ref</t>
   </si>
   <si>
     <t xml:space="preserve">status</t>
@@ -1220,10 +1217,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:G234"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A211" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E231" activeCellId="0" sqref="E231"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1253,16 +1250,10 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1273,7 +1264,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1284,7 +1275,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1295,1644 +1286,1351 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>30</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G15" s="3" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>7</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G17" s="3" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="G21" s="3" t="n">
-        <v>2</v>
+        <v>25</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="C26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="G27" s="3"/>
+        <v>32</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="4" t="s">
+      <c r="E30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="1" t="s">
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="3" t="n">
+      <c r="B33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F33" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G33" s="3"/>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G37" s="1" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G40" s="1" t="n">
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G42" s="3"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F43" s="3" t="n">
-        <v>35</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" s="3" t="n">
-        <v>300</v>
-      </c>
-      <c r="G47" s="3"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F48" s="3" t="n">
-        <v>35</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G51" s="1" t="n">
-        <v>2</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G52" s="1" t="n">
-        <v>4</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G53" s="1" t="n">
-        <v>2</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G54" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G57" s="1" t="n">
-        <v>3</v>
-      </c>
+      <c r="C57" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F58" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="G58" s="3"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G61" s="1" t="n">
-        <v>15</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G62" s="1" t="n">
-        <v>15</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G63" s="1" t="n">
-        <v>15</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C65" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F64" s="3" t="n">
+      <c r="B67" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G64" s="3" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F67" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G67" s="3"/>
+      <c r="D67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F68" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F68" s="3"/>
       <c r="G68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F69" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F69" s="3"/>
       <c r="G69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F70" s="3" t="n">
-        <v>20</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F70" s="3"/>
       <c r="G70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F72" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="G72" s="3"/>
+        <v>74</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F73" s="3" t="n">
-        <v>20</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F73" s="3"/>
       <c r="G73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G74" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F75" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="G75" s="3"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F76" s="3" t="n">
-        <v>10</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F76" s="3"/>
       <c r="G76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G79" s="1" t="n">
-        <v>2</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F80" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G80" s="3"/>
+        <v>81</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G82" s="1" t="n">
-        <v>2</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G83" s="1" t="n">
-        <v>2</v>
+        <v>84</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G84" s="1" t="n">
-        <v>2</v>
+        <v>85</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G85" s="1" t="n">
-        <v>2</v>
+        <v>86</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G86" s="1" t="n">
-        <v>2</v>
+        <v>61</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C88" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D89" s="3"/>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F90" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G90" s="3"/>
+      <c r="C90" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F91" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="F91" s="3"/>
       <c r="G91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F92" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F92" s="3"/>
       <c r="G92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F93" s="3" t="n">
-        <v>30</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="F93" s="3"/>
       <c r="G93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="1" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F96" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G96" s="3"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G98" s="1" t="n">
-        <v>2</v>
+        <v>80</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F99" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G99" s="3"/>
+        <v>81</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="1" t="s">
-        <v>95</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G102" s="1" t="n">
-        <v>2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G103" s="1" t="n">
-        <v>2</v>
+        <v>84</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F104" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G104" s="3"/>
+        <v>85</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G105" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F106" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="G106" s="3"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="1" t="s">
-        <v>99</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C113" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="114" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B114" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D114" s="4"/>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C115" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F115" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G115" s="3"/>
+      <c r="C115" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D115" s="4"/>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C116" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F116" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="F116" s="3"/>
       <c r="G116" s="3"/>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C117" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F117" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F117" s="3"/>
       <c r="G117" s="3"/>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D118" s="5"/>
-      <c r="G118" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="C118" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F119" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="G119" s="3"/>
+      <c r="C119" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D119" s="5"/>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C120" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F120" s="3"/>
+      <c r="G120" s="3"/>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="1" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C122" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F122" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G122" s="3"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C123" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F124" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G124" s="3"/>
+        <v>80</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C125" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C126" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F125" s="3"/>
+      <c r="G125" s="3"/>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C126" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C127" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D127" s="4"/>
+      <c r="E127" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
+    </row>
+    <row r="128" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C128" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D126" s="4"/>
-      <c r="E126" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F126" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G126" s="3"/>
-    </row>
-    <row r="127" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="4" t="s">
+      <c r="D128" s="4"/>
+    </row>
+    <row r="129" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C129" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D127" s="4"/>
-    </row>
-    <row r="128" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C128" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D128" s="4"/>
-    </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C129" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="D129" s="4"/>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G130" s="1" t="n">
-        <v>3</v>
+        <v>84</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G131" s="1" t="n">
-        <v>2</v>
+        <v>85</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C132" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C133" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G132" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="3" t="s">
+      <c r="B135" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B134" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C134" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D134" s="4"/>
-    </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C135" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F135" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G135" s="3"/>
+      <c r="C135" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D135" s="4"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F136" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F136" s="3"/>
       <c r="G136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F137" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F137" s="3"/>
       <c r="G137" s="3"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C138" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D138" s="5"/>
+      <c r="C138" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C139" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F139" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="G139" s="3"/>
+      <c r="C139" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D139" s="5"/>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F140" s="3"/>
+      <c r="G140" s="3"/>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F142" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G142" s="3"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C143" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F143" s="3" t="n">
-        <v>35</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F143" s="3"/>
       <c r="G143" s="3"/>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C144" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G144" s="1" t="n">
-        <v>2</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F144" s="3"/>
+      <c r="G144" s="3"/>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C145" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G145" s="1" t="n">
-        <v>2</v>
+        <v>113</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G146" s="1" t="n">
-        <v>2</v>
+        <v>114</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C147" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G147" s="1" t="n">
-        <v>2</v>
+        <v>115</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C148" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C149" s="1" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C151" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C152" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="151" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D151" s="4"/>
-    </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C152" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G152" s="1" t="n">
-        <v>3</v>
-      </c>
+      <c r="D152" s="4"/>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C153" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G153" s="1" t="n">
-        <v>3</v>
+        <v>120</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C154" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G154" s="1" t="n">
-        <v>3</v>
+        <v>121</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C155" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G155" s="1" t="n">
-        <v>3</v>
+        <v>122</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C156" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G156" s="1" t="n">
-        <v>3</v>
+        <v>123</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F157" s="3" t="n">
-        <v>500</v>
-      </c>
-      <c r="G157" s="3"/>
+        <v>124</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F158" s="3"/>
+      <c r="G158" s="3"/>
+    </row>
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C159" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="160" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="3" t="s">
+      <c r="B161" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B160" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C160" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D160" s="4"/>
-    </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C161" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F161" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G161" s="3"/>
+      <c r="C161" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D161" s="4"/>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C162" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F162" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F162" s="3"/>
       <c r="G162" s="3"/>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C163" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F163" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F163" s="3"/>
       <c r="G163" s="3"/>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C164" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F164" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="F164" s="3"/>
       <c r="G164" s="3"/>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C165" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F165" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="F165" s="3"/>
       <c r="G165" s="3"/>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F166" s="3" t="n">
-        <v>30</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="F166" s="3"/>
       <c r="G166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C167" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F167" s="3"/>
+      <c r="G167" s="3"/>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C168" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F168" s="4"/>
-      <c r="G168" s="4"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C169" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F169" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G169" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="F169" s="4"/>
+      <c r="G169" s="4"/>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C170" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F170" s="3" t="n">
-        <v>35</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F170" s="3"/>
       <c r="G170" s="3"/>
     </row>
-    <row r="171" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C171" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D171" s="4"/>
-    </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C172" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F172" s="3" t="n">
-        <v>500</v>
-      </c>
-      <c r="G172" s="3"/>
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C171" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F171" s="3"/>
+      <c r="G171" s="3"/>
+    </row>
+    <row r="172" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C172" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D172" s="4"/>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C173" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F173" s="3"/>
+      <c r="G173" s="3"/>
+    </row>
+    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C174" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="175" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="3" t="s">
+      <c r="B176" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B175" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C175" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D175" s="4"/>
-    </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C176" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F176" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G176" s="3"/>
+      <c r="C176" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D176" s="4"/>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C177" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F177" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F177" s="3"/>
       <c r="G177" s="3"/>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D178" s="5"/>
+      <c r="C178" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F178" s="3"/>
+      <c r="G178" s="3"/>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C179" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F179" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="G179" s="3"/>
+      <c r="C179" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D179" s="5"/>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C180" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F180" s="3" t="n">
-        <v>30</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F180" s="3"/>
       <c r="G180" s="3"/>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C181" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="F181" s="3"/>
+      <c r="G181" s="3"/>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C182" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C183" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F183" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G183" s="3"/>
-    </row>
-    <row r="184" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C184" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D184" s="4"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C184" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F184" s="3"/>
+      <c r="G184" s="3"/>
     </row>
     <row r="185" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C185" s="4" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="D185" s="4"/>
     </row>
-    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C186" s="1" t="s">
+    <row r="186" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C186" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D186" s="4"/>
+    </row>
+    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C187" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="188" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="3" t="s">
+      <c r="B189" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B188" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C188" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D188" s="4"/>
-    </row>
-    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C189" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F189" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G189" s="3"/>
+      <c r="C189" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D189" s="4"/>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C190" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F190" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F190" s="3"/>
       <c r="G190" s="3"/>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C191" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F191" s="3" t="n">
-        <v>70</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F191" s="3"/>
       <c r="G191" s="3"/>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C192" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D192" s="5"/>
+      <c r="C192" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F192" s="3"/>
+      <c r="G192" s="3"/>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C193" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F193" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="G193" s="3"/>
+      <c r="C193" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D193" s="5"/>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C194" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F194" s="3"/>
+      <c r="G194" s="3"/>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C195" s="1" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C196" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C197" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F197" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G197" s="3"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C198" s="1" t="s">
-        <v>140</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F198" s="3"/>
+      <c r="G198" s="3"/>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C199" s="1" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C200" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C201" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G201" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="203" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C202" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B204" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B203" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C203" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D203" s="4"/>
-    </row>
-    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C204" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F204" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="G204" s="3"/>
+      <c r="C204" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D204" s="4"/>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C205" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F205" s="3" t="n">
-        <v>30</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="F205" s="3"/>
       <c r="G205" s="3"/>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C206" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F206" s="3"/>
+      <c r="G206" s="3"/>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C207" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F207" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G207" s="3"/>
+        <v>143</v>
+      </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C208" s="1" t="s">
-        <v>146</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F208" s="3"/>
+      <c r="G208" s="3"/>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C209" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C210" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B212" s="3" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B211" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D211" s="3"/>
-    </row>
-    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C212" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F212" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="G212" s="3"/>
+      <c r="C212" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D212" s="3"/>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C213" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F213" s="3" t="n">
-        <v>50</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F213" s="3"/>
       <c r="G213" s="3"/>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C214" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F214" s="3" t="n">
-        <v>50</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="F214" s="3"/>
       <c r="G214" s="3"/>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C215" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F215" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="G215" s="3" t="n">
-        <v>3</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="F215" s="3"/>
+      <c r="G215" s="3"/>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C216" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F216" s="3"/>
+      <c r="G216" s="3"/>
+    </row>
+    <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C217" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="3" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="3" t="s">
+      <c r="B219" s="3"/>
+      <c r="C219" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B218" s="3"/>
-      <c r="C218" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D218" s="3"/>
-      <c r="F218" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="G218" s="3"/>
-    </row>
-    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C219" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F219" s="3" t="n">
-        <v>70</v>
-      </c>
+      <c r="D219" s="3"/>
+      <c r="F219" s="3"/>
       <c r="G219" s="3"/>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C220" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F220" s="1" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B222" s="3"/>
-      <c r="C222" s="3"/>
-      <c r="D222" s="3"/>
-      <c r="E222" s="3"/>
-      <c r="F222" s="3"/>
-      <c r="G222" s="3"/>
+        <v>154</v>
+      </c>
+      <c r="F220" s="3"/>
+      <c r="G220" s="3"/>
+    </row>
+    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C221" s="1" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
@@ -2943,7 +2641,7 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B224" s="3"/>
       <c r="C224" s="3"/>
@@ -2954,7 +2652,7 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B225" s="3"/>
       <c r="C225" s="3"/>
@@ -2964,99 +2662,104 @@
       <c r="G225" s="3"/>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="2" t="s">
+      <c r="A226" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B226" s="3"/>
+      <c r="C226" s="3"/>
+      <c r="D226" s="3"/>
+      <c r="E226" s="3"/>
+      <c r="F226" s="3"/>
+      <c r="G226" s="3"/>
+    </row>
+    <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B227" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B227" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="E227" s="3" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E230" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E232" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B233" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B234" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B233" s="6" t="s">
+      <c r="E234" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E233" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E7:E219" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E7:E220" type="list">
       <formula1>Datatypes!$A$2:$A$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3076,17 +2779,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3096,59 +2799,38 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3" t="n">
-        <v>30</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3166,17 +2848,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,26 +2868,18 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3223,17 +2897,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3243,50 +2917,32 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="n">
-        <v>30</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3304,17 +2960,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3324,59 +2980,38 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3" t="n">
-        <v>10</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3" t="n">
-        <v>30</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3394,17 +3029,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3414,54 +3049,32 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3" t="n">
-        <v>50</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="n">
-        <v>5000</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3479,17 +3092,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3499,26 +3112,18 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3536,17 +3141,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E231 A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3556,54 +3161,33 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>10</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>30</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>70</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>30</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3622,17 +3206,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="43.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3642,127 +3226,106 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>500</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>2</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>100</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -3781,17 +3344,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E231 B1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3801,196 +3364,133 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>10</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C9" s="3" t="n">
-        <v>10</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>20</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="3" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>10</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C14" s="3" t="n">
-        <v>10</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C15" s="3" t="n">
-        <v>20</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C16" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>7</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C17" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>4</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="C18" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="D18" s="3" t="n">
-        <v>4</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="3" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -4009,17 +3509,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="E231 A9"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4029,67 +3529,37 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>194</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>256</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4106,18 +3576,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E231 A2"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4127,64 +3596,38 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>35</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="n">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -4211,7 +3654,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="E231 A8"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4221,48 +3664,48 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -4281,17 +3724,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="E231 A6"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4301,53 +3744,36 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3" t="n">
-        <v>50</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4365,17 +3791,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E231 A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4385,73 +3811,48 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="3" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="3" t="n">
-        <v>100</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4469,15 +3870,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E231 A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4487,58 +3889,41 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4556,17 +3941,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E231 A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4576,31 +3961,18 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3" t="n">
-        <v>500</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4618,17 +3990,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="E231 A5"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4638,48 +4010,30 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3" t="n">
-        <v>50</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="n">
-        <v>100</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4697,17 +4051,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="E231 C11"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4717,33 +4071,21 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -4762,17 +4104,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="E231 C7"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4782,51 +4124,30 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3" t="n">
-        <v>250</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="n">
-        <v>50</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>